<commit_message>
Updated word and excel templates
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12CFBF6-5F88-41BD-8516-4E1BE1A541DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+  <si>
+    <t>Summary / Title</t>
+  </si>
+  <si>
+    <t>Initial Conditions</t>
+  </si>
+  <si>
+    <t>Internet connection</t>
+  </si>
+  <si>
+    <t>Internet Explorer 6 or greater</t>
+  </si>
+  <si>
+    <t>EXECUTION</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>PASS / FAIL</t>
+  </si>
+  <si>
+    <t>Access the website home page</t>
+  </si>
+  <si>
+    <t>Display the home web page</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Click the home button</t>
+  </si>
+  <si>
+    <t>Display the home web page with a reload</t>
+  </si>
+  <si>
+    <t>Post Conditions</t>
+  </si>
+  <si>
+    <t>The browser display the home page</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +93,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -45,15 +144,271 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7198AF8C-278E-4D19-8806-A09E05ED7257}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +685,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="3">
+        <v>1</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:G10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed word document template and added one manual testing test case
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21A0E26-EC44-424B-88B9-C963C90FA96B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2623A262-CC8D-4CA6-A64B-E86D65CC8E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
+    <sheet name="Testarea funcțională" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -810,15 +810,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,6 +844,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1153,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1169,10 +1169,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="6">
         <v>1</v>
       </c>
@@ -1181,10 +1181,10 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1193,36 +1193,36 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
@@ -1326,10 +1326,10 @@
     </row>
     <row r="14" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="15" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
@@ -1338,10 +1338,10 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6" t="s">
         <v>93</v>
       </c>
@@ -1350,26 +1350,26 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="23" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="26"/>
@@ -1382,14 +1382,14 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
@@ -1493,10 +1493,10 @@
     </row>
     <row r="28" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="29" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="6">
         <v>3</v>
       </c>
@@ -1505,10 +1505,10 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="6" t="s">
         <v>94</v>
       </c>
@@ -1517,36 +1517,36 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="23" t="s">
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="1" t="s">
@@ -1664,10 +1664,10 @@
     </row>
     <row r="42" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="43" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="6">
         <v>4</v>
       </c>
@@ -1676,10 +1676,10 @@
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="6" t="s">
         <v>95</v>
       </c>
@@ -1688,36 +1688,36 @@
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="20" t="s">
+      <c r="C45" s="14"/>
+      <c r="D45" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="23" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="25"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="13"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B48" s="1" t="s">
@@ -1821,10 +1821,10 @@
     </row>
     <row r="55" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="56" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="15"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="6">
         <v>5</v>
       </c>
@@ -1833,10 +1833,10 @@
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="15"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="6" t="s">
         <v>51</v>
       </c>
@@ -1845,36 +1845,36 @@
       <c r="G57" s="7"/>
     </row>
     <row r="58" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="14"/>
+      <c r="D58" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="22"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="23" t="s">
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="25"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="22"/>
     </row>
     <row r="60" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="13"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="25"/>
     </row>
     <row r="61" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B61" s="1" t="s">
@@ -1978,10 +1978,10 @@
     </row>
     <row r="68" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="69" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="15"/>
+      <c r="C69" s="12"/>
       <c r="D69" s="6">
         <v>6</v>
       </c>
@@ -1990,10 +1990,10 @@
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="15"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="6" t="s">
         <v>79</v>
       </c>
@@ -2002,36 +2002,36 @@
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="20" t="s">
+      <c r="C71" s="14"/>
+      <c r="D71" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="22"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="19"/>
     </row>
     <row r="72" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="23" t="s">
+      <c r="B72" s="15"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="25"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="22"/>
     </row>
     <row r="73" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="13"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="25"/>
     </row>
     <row r="74" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B74" s="1" t="s">
@@ -2149,10 +2149,10 @@
     </row>
     <row r="82" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="83" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="15"/>
+      <c r="C83" s="12"/>
       <c r="D83" s="6">
         <v>7</v>
       </c>
@@ -2161,10 +2161,10 @@
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="15"/>
+      <c r="C84" s="12"/>
       <c r="D84" s="6" t="s">
         <v>66</v>
       </c>
@@ -2173,36 +2173,36 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="20" t="s">
+      <c r="C85" s="14"/>
+      <c r="D85" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="22"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="23" t="s">
+      <c r="B86" s="15"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="25"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="22"/>
     </row>
     <row r="87" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="13"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="25"/>
     </row>
     <row r="88" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B88" s="1" t="s">
@@ -2292,10 +2292,10 @@
     </row>
     <row r="94" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="95" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="15"/>
+      <c r="C95" s="12"/>
       <c r="D95" s="6">
         <v>8</v>
       </c>
@@ -2304,10 +2304,10 @@
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="15"/>
+      <c r="C96" s="12"/>
       <c r="D96" s="6" t="s">
         <v>96</v>
       </c>
@@ -2316,36 +2316,36 @@
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="20" t="s">
+      <c r="C97" s="14"/>
+      <c r="D97" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="22"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="19"/>
     </row>
     <row r="98" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B98" s="18"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="23" t="s">
+      <c r="B98" s="15"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="25"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="22"/>
     </row>
     <row r="99" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="13"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="25"/>
     </row>
     <row r="100" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B100" s="1" t="s">
@@ -2435,10 +2435,10 @@
     </row>
     <row r="106" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="107" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="15"/>
+      <c r="C107" s="12"/>
       <c r="D107" s="6">
         <v>9</v>
       </c>
@@ -2447,10 +2447,10 @@
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="15"/>
+      <c r="C108" s="12"/>
       <c r="D108" s="6" t="s">
         <v>106</v>
       </c>
@@ -2459,36 +2459,36 @@
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C109" s="17"/>
-      <c r="D109" s="20" t="s">
+      <c r="C109" s="14"/>
+      <c r="D109" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E109" s="21"/>
-      <c r="F109" s="21"/>
-      <c r="G109" s="22"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="19"/>
     </row>
     <row r="110" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B110" s="18"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="23" t="s">
+      <c r="B110" s="15"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E110" s="24"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="25"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="22"/>
     </row>
     <row r="111" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="13"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="25"/>
     </row>
     <row r="112" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B112" s="1" t="s">
@@ -2578,10 +2578,10 @@
     </row>
     <row r="118" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="119" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="15"/>
+      <c r="C119" s="12"/>
       <c r="D119" s="6">
         <v>10</v>
       </c>
@@ -2590,10 +2590,10 @@
       <c r="G119" s="7"/>
     </row>
     <row r="120" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="15"/>
+      <c r="C120" s="12"/>
       <c r="D120" s="6" t="s">
         <v>117</v>
       </c>
@@ -2602,36 +2602,36 @@
       <c r="G120" s="7"/>
     </row>
     <row r="121" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C121" s="17"/>
-      <c r="D121" s="20" t="s">
+      <c r="C121" s="14"/>
+      <c r="D121" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
-      <c r="G121" s="22"/>
+      <c r="E121" s="18"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="19"/>
     </row>
     <row r="122" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B122" s="18"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="23" t="s">
+      <c r="B122" s="15"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E122" s="24"/>
-      <c r="F122" s="24"/>
-      <c r="G122" s="25"/>
+      <c r="E122" s="21"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="22"/>
     </row>
     <row r="123" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-      <c r="G123" s="13"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="25"/>
     </row>
     <row r="124" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B124" s="1" t="s">
@@ -2791,10 +2791,10 @@
     </row>
     <row r="135" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="136" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C136" s="15"/>
+      <c r="C136" s="12"/>
       <c r="D136" s="6">
         <v>11</v>
       </c>
@@ -2803,10 +2803,10 @@
       <c r="G136" s="7"/>
     </row>
     <row r="137" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B137" s="14" t="s">
+      <c r="B137" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="15"/>
+      <c r="C137" s="12"/>
       <c r="D137" s="6" t="s">
         <v>147</v>
       </c>
@@ -2815,36 +2815,36 @@
       <c r="G137" s="7"/>
     </row>
     <row r="138" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B138" s="16" t="s">
+      <c r="B138" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C138" s="17"/>
-      <c r="D138" s="20" t="s">
+      <c r="C138" s="14"/>
+      <c r="D138" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E138" s="21"/>
-      <c r="F138" s="21"/>
-      <c r="G138" s="22"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="18"/>
+      <c r="G138" s="19"/>
     </row>
     <row r="139" spans="2:7" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B139" s="18"/>
-      <c r="C139" s="19"/>
-      <c r="D139" s="23" t="s">
+      <c r="B139" s="15"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E139" s="24"/>
-      <c r="F139" s="24"/>
-      <c r="G139" s="25"/>
+      <c r="E139" s="21"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="22"/>
     </row>
     <row r="140" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B140" s="11" t="s">
+      <c r="B140" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C140" s="12"/>
-      <c r="D140" s="12"/>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
-      <c r="G140" s="13"/>
+      <c r="C140" s="24"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="24"/>
+      <c r="G140" s="25"/>
     </row>
     <row r="141" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B141" s="1" t="s">
@@ -2962,10 +2962,10 @@
     </row>
     <row r="149" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="150" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B150" s="14" t="s">
+      <c r="B150" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="15"/>
+      <c r="C150" s="12"/>
       <c r="D150" s="6">
         <v>12</v>
       </c>
@@ -2974,10 +2974,10 @@
       <c r="G150" s="7"/>
     </row>
     <row r="151" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B151" s="14" t="s">
+      <c r="B151" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="15"/>
+      <c r="C151" s="12"/>
       <c r="D151" s="6" t="s">
         <v>137</v>
       </c>
@@ -2986,36 +2986,36 @@
       <c r="G151" s="7"/>
     </row>
     <row r="152" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B152" s="16" t="s">
+      <c r="B152" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C152" s="17"/>
-      <c r="D152" s="20" t="s">
+      <c r="C152" s="14"/>
+      <c r="D152" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E152" s="21"/>
-      <c r="F152" s="21"/>
-      <c r="G152" s="22"/>
+      <c r="E152" s="18"/>
+      <c r="F152" s="18"/>
+      <c r="G152" s="19"/>
     </row>
     <row r="153" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B153" s="18"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="23" t="s">
+      <c r="B153" s="15"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E153" s="24"/>
-      <c r="F153" s="24"/>
-      <c r="G153" s="25"/>
+      <c r="E153" s="21"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="22"/>
     </row>
     <row r="154" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
-      <c r="G154" s="13"/>
+      <c r="C154" s="24"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="24"/>
+      <c r="F154" s="24"/>
+      <c r="G154" s="25"/>
     </row>
     <row r="155" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B155" s="1" t="s">
@@ -3120,72 +3120,113 @@
     <row r="162" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="197">
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="D151:G151"/>
-    <mergeCell ref="B152:C153"/>
-    <mergeCell ref="D152:G152"/>
-    <mergeCell ref="D153:G153"/>
-    <mergeCell ref="B154:G154"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="D137:G137"/>
-    <mergeCell ref="B138:C139"/>
-    <mergeCell ref="D138:G138"/>
-    <mergeCell ref="D139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="B123:G123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:G134"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="D136:G136"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:G117"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="B121:C122"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="D122:G122"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:G108"/>
-    <mergeCell ref="B109:C110"/>
-    <mergeCell ref="D109:G109"/>
-    <mergeCell ref="D110:G110"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D105:G105"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B99:G99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="B97:C98"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="D98:G98"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="D93:G93"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B71:C72"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B17:C19"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="B3:C3"/>
@@ -3210,113 +3251,72 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B71:C72"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D105:G105"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="B99:G99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:G96"/>
-    <mergeCell ref="B97:C98"/>
-    <mergeCell ref="D97:G97"/>
-    <mergeCell ref="D98:G98"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="D93:G93"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:G95"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:G108"/>
+    <mergeCell ref="B109:C110"/>
+    <mergeCell ref="D109:G109"/>
+    <mergeCell ref="D110:G110"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="B121:C122"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="D122:G122"/>
+    <mergeCell ref="B123:G123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:G134"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="D136:G136"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="D137:G137"/>
+    <mergeCell ref="B138:C139"/>
+    <mergeCell ref="D138:G138"/>
+    <mergeCell ref="D139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="D151:G151"/>
+    <mergeCell ref="B152:C153"/>
+    <mergeCell ref="D152:G152"/>
+    <mergeCell ref="D153:G153"/>
+    <mergeCell ref="B154:G154"/>
+    <mergeCell ref="C155:D155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the other manual test case for maxi-pet and updated the excel
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2623A262-CC8D-4CA6-A64B-E86D65CC8E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D2FB28-7EA7-4D61-9486-B7AC1EF893FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="160">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -502,6 +502,9 @@
   </si>
   <si>
     <t>Sunt afișate toate produsele din brand-ul primei cuști pentru iepuri care apare pe website</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -808,6 +811,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -846,15 +858,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -869,6 +872,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1153,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1169,10 +1175,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="6">
         <v>1</v>
       </c>
@@ -1181,10 +1187,10 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1193,36 +1199,36 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="20" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="7" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
@@ -1326,10 +1332,10 @@
     </row>
     <row r="14" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="15" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
@@ -1338,10 +1344,10 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="6" t="s">
         <v>93</v>
       </c>
@@ -1350,26 +1356,26 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="17"/>
+      <c r="D17" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="19"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="20" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="26"/>
@@ -1382,14 +1388,14 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
@@ -1493,10 +1499,10 @@
     </row>
     <row r="28" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="29" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="15"/>
       <c r="D29" s="6">
         <v>3</v>
       </c>
@@ -1505,10 +1511,10 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="15"/>
       <c r="D30" s="6" t="s">
         <v>94</v>
       </c>
@@ -1517,36 +1523,36 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="17" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="19"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
     </row>
     <row r="32" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="20" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="1" t="s">
@@ -1664,10 +1670,10 @@
     </row>
     <row r="42" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="43" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="12"/>
+      <c r="C43" s="15"/>
       <c r="D43" s="6">
         <v>4</v>
       </c>
@@ -1676,10 +1682,10 @@
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="15"/>
       <c r="D44" s="6" t="s">
         <v>95</v>
       </c>
@@ -1688,36 +1694,36 @@
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="17" t="s">
+      <c r="C45" s="17"/>
+      <c r="D45" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="19"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="15"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="20" t="s">
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="25"/>
     </row>
     <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="23" t="s">
+      <c r="B47" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="25"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="13"/>
     </row>
     <row r="48" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B48" s="1" t="s">
@@ -1821,10 +1827,10 @@
     </row>
     <row r="55" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="56" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="12"/>
+      <c r="C56" s="15"/>
       <c r="D56" s="6">
         <v>5</v>
       </c>
@@ -1833,10 +1839,10 @@
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="15"/>
       <c r="D57" s="6" t="s">
         <v>51</v>
       </c>
@@ -1845,36 +1851,36 @@
       <c r="G57" s="7"/>
     </row>
     <row r="58" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="17" t="s">
+      <c r="C58" s="17"/>
+      <c r="D58" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="19"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="22"/>
     </row>
     <row r="59" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B59" s="15"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="20" t="s">
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="22"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="25"/>
     </row>
     <row r="60" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B60" s="23" t="s">
+      <c r="B60" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="25"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="13"/>
     </row>
     <row r="61" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B61" s="1" t="s">
@@ -1978,10 +1984,10 @@
     </row>
     <row r="68" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="69" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="12"/>
+      <c r="C69" s="15"/>
       <c r="D69" s="6">
         <v>6</v>
       </c>
@@ -1990,10 +1996,10 @@
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B70" s="11" t="s">
+      <c r="B70" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="12"/>
+      <c r="C70" s="15"/>
       <c r="D70" s="6" t="s">
         <v>79</v>
       </c>
@@ -2002,36 +2008,36 @@
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="17" t="s">
+      <c r="C71" s="17"/>
+      <c r="D71" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="19"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="22"/>
     </row>
     <row r="72" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B72" s="15"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="20" t="s">
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="22"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="25"/>
     </row>
     <row r="73" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="25"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="13"/>
     </row>
     <row r="74" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B74" s="1" t="s">
@@ -2149,10 +2155,10 @@
     </row>
     <row r="82" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="83" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="12"/>
+      <c r="C83" s="15"/>
       <c r="D83" s="6">
         <v>7</v>
       </c>
@@ -2161,10 +2167,10 @@
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="12"/>
+      <c r="C84" s="15"/>
       <c r="D84" s="6" t="s">
         <v>66</v>
       </c>
@@ -2173,36 +2179,36 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B85" s="13" t="s">
+      <c r="B85" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="14"/>
-      <c r="D85" s="17" t="s">
+      <c r="C85" s="17"/>
+      <c r="D85" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="19"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="22"/>
     </row>
     <row r="86" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B86" s="15"/>
-      <c r="C86" s="16"/>
-      <c r="D86" s="20" t="s">
+      <c r="B86" s="18"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="E86" s="21"/>
-      <c r="F86" s="21"/>
-      <c r="G86" s="22"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="25"/>
     </row>
     <row r="87" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B87" s="23" t="s">
+      <c r="B87" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="25"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="13"/>
     </row>
     <row r="88" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B88" s="1" t="s">
@@ -2292,10 +2298,10 @@
     </row>
     <row r="94" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="95" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B95" s="11" t="s">
+      <c r="B95" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="12"/>
+      <c r="C95" s="15"/>
       <c r="D95" s="6">
         <v>8</v>
       </c>
@@ -2304,10 +2310,10 @@
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B96" s="11" t="s">
+      <c r="B96" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="12"/>
+      <c r="C96" s="15"/>
       <c r="D96" s="6" t="s">
         <v>96</v>
       </c>
@@ -2316,36 +2322,36 @@
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B97" s="13" t="s">
+      <c r="B97" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C97" s="14"/>
-      <c r="D97" s="17" t="s">
+      <c r="C97" s="17"/>
+      <c r="D97" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E97" s="18"/>
-      <c r="F97" s="18"/>
-      <c r="G97" s="19"/>
+      <c r="E97" s="21"/>
+      <c r="F97" s="21"/>
+      <c r="G97" s="22"/>
     </row>
     <row r="98" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B98" s="15"/>
-      <c r="C98" s="16"/>
-      <c r="D98" s="20" t="s">
+      <c r="B98" s="18"/>
+      <c r="C98" s="19"/>
+      <c r="D98" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
-      <c r="G98" s="22"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="25"/>
     </row>
     <row r="99" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B99" s="23" t="s">
+      <c r="B99" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="24"/>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="25"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="13"/>
     </row>
     <row r="100" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B100" s="1" t="s">
@@ -2435,10 +2441,10 @@
     </row>
     <row r="106" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="107" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B107" s="11" t="s">
+      <c r="B107" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="12"/>
+      <c r="C107" s="15"/>
       <c r="D107" s="6">
         <v>9</v>
       </c>
@@ -2447,10 +2453,10 @@
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B108" s="11" t="s">
+      <c r="B108" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="12"/>
+      <c r="C108" s="15"/>
       <c r="D108" s="6" t="s">
         <v>106</v>
       </c>
@@ -2459,36 +2465,36 @@
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B109" s="13" t="s">
+      <c r="B109" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C109" s="14"/>
-      <c r="D109" s="17" t="s">
+      <c r="C109" s="17"/>
+      <c r="D109" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E109" s="18"/>
-      <c r="F109" s="18"/>
-      <c r="G109" s="19"/>
+      <c r="E109" s="21"/>
+      <c r="F109" s="21"/>
+      <c r="G109" s="22"/>
     </row>
     <row r="110" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B110" s="15"/>
-      <c r="C110" s="16"/>
-      <c r="D110" s="20" t="s">
+      <c r="B110" s="18"/>
+      <c r="C110" s="19"/>
+      <c r="D110" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E110" s="21"/>
-      <c r="F110" s="21"/>
-      <c r="G110" s="22"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="25"/>
     </row>
     <row r="111" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B111" s="23" t="s">
+      <c r="B111" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C111" s="24"/>
-      <c r="D111" s="24"/>
-      <c r="E111" s="24"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="25"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12"/>
+      <c r="G111" s="13"/>
     </row>
     <row r="112" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B112" s="1" t="s">
@@ -2519,8 +2525,12 @@
       <c r="E113" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F113" s="4"/>
-      <c r="G113" s="5"/>
+      <c r="F113" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G113" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="114" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B114" s="3">
@@ -2533,8 +2543,12 @@
       <c r="E114" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F114" s="4"/>
-      <c r="G114" s="5"/>
+      <c r="F114" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G114" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="115" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B115" s="3">
@@ -2547,8 +2561,12 @@
       <c r="E115" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F115" s="4"/>
-      <c r="G115" s="5"/>
+      <c r="F115" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G115" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="116" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B116" s="3">
@@ -2561,8 +2579,12 @@
       <c r="E116" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F116" s="4"/>
-      <c r="G116" s="5"/>
+      <c r="F116" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G116" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="117" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B117" s="8" t="s">
@@ -2578,10 +2600,10 @@
     </row>
     <row r="118" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="119" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="12"/>
+      <c r="C119" s="15"/>
       <c r="D119" s="6">
         <v>10</v>
       </c>
@@ -2590,10 +2612,10 @@
       <c r="G119" s="7"/>
     </row>
     <row r="120" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B120" s="11" t="s">
+      <c r="B120" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="12"/>
+      <c r="C120" s="15"/>
       <c r="D120" s="6" t="s">
         <v>117</v>
       </c>
@@ -2602,36 +2624,36 @@
       <c r="G120" s="7"/>
     </row>
     <row r="121" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B121" s="13" t="s">
+      <c r="B121" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C121" s="14"/>
-      <c r="D121" s="17" t="s">
+      <c r="C121" s="17"/>
+      <c r="D121" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E121" s="18"/>
-      <c r="F121" s="18"/>
-      <c r="G121" s="19"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="21"/>
+      <c r="G121" s="22"/>
     </row>
     <row r="122" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B122" s="15"/>
-      <c r="C122" s="16"/>
-      <c r="D122" s="20" t="s">
+      <c r="B122" s="18"/>
+      <c r="C122" s="19"/>
+      <c r="D122" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E122" s="21"/>
-      <c r="F122" s="21"/>
-      <c r="G122" s="22"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="24"/>
+      <c r="G122" s="25"/>
     </row>
     <row r="123" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B123" s="23" t="s">
+      <c r="B123" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C123" s="24"/>
-      <c r="D123" s="24"/>
-      <c r="E123" s="24"/>
-      <c r="F123" s="24"/>
-      <c r="G123" s="25"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12"/>
+      <c r="G123" s="13"/>
     </row>
     <row r="124" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B124" s="1" t="s">
@@ -2791,10 +2813,10 @@
     </row>
     <row r="135" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="136" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B136" s="11" t="s">
+      <c r="B136" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C136" s="12"/>
+      <c r="C136" s="15"/>
       <c r="D136" s="6">
         <v>11</v>
       </c>
@@ -2803,10 +2825,10 @@
       <c r="G136" s="7"/>
     </row>
     <row r="137" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="12"/>
+      <c r="C137" s="15"/>
       <c r="D137" s="6" t="s">
         <v>147</v>
       </c>
@@ -2815,36 +2837,36 @@
       <c r="G137" s="7"/>
     </row>
     <row r="138" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B138" s="13" t="s">
+      <c r="B138" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C138" s="14"/>
-      <c r="D138" s="17" t="s">
+      <c r="C138" s="17"/>
+      <c r="D138" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E138" s="18"/>
-      <c r="F138" s="18"/>
-      <c r="G138" s="19"/>
+      <c r="E138" s="21"/>
+      <c r="F138" s="21"/>
+      <c r="G138" s="22"/>
     </row>
     <row r="139" spans="2:7" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B139" s="15"/>
-      <c r="C139" s="16"/>
-      <c r="D139" s="20" t="s">
+      <c r="B139" s="18"/>
+      <c r="C139" s="19"/>
+      <c r="D139" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E139" s="21"/>
-      <c r="F139" s="21"/>
-      <c r="G139" s="22"/>
+      <c r="E139" s="24"/>
+      <c r="F139" s="24"/>
+      <c r="G139" s="25"/>
     </row>
     <row r="140" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B140" s="23" t="s">
+      <c r="B140" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C140" s="24"/>
-      <c r="D140" s="24"/>
-      <c r="E140" s="24"/>
-      <c r="F140" s="24"/>
-      <c r="G140" s="25"/>
+      <c r="C140" s="12"/>
+      <c r="D140" s="12"/>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="13"/>
     </row>
     <row r="141" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B141" s="1" t="s">
@@ -2962,10 +2984,10 @@
     </row>
     <row r="149" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="150" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="12"/>
+      <c r="C150" s="15"/>
       <c r="D150" s="6">
         <v>12</v>
       </c>
@@ -2974,10 +2996,10 @@
       <c r="G150" s="7"/>
     </row>
     <row r="151" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B151" s="11" t="s">
+      <c r="B151" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="12"/>
+      <c r="C151" s="15"/>
       <c r="D151" s="6" t="s">
         <v>137</v>
       </c>
@@ -2986,36 +3008,36 @@
       <c r="G151" s="7"/>
     </row>
     <row r="152" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B152" s="13" t="s">
+      <c r="B152" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C152" s="14"/>
-      <c r="D152" s="17" t="s">
+      <c r="C152" s="17"/>
+      <c r="D152" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E152" s="18"/>
-      <c r="F152" s="18"/>
-      <c r="G152" s="19"/>
+      <c r="E152" s="21"/>
+      <c r="F152" s="21"/>
+      <c r="G152" s="22"/>
     </row>
     <row r="153" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B153" s="15"/>
-      <c r="C153" s="16"/>
-      <c r="D153" s="20" t="s">
+      <c r="B153" s="18"/>
+      <c r="C153" s="19"/>
+      <c r="D153" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E153" s="21"/>
-      <c r="F153" s="21"/>
-      <c r="G153" s="22"/>
+      <c r="E153" s="24"/>
+      <c r="F153" s="24"/>
+      <c r="G153" s="25"/>
     </row>
     <row r="154" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B154" s="23" t="s">
+      <c r="B154" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C154" s="24"/>
-      <c r="D154" s="24"/>
-      <c r="E154" s="24"/>
-      <c r="F154" s="24"/>
-      <c r="G154" s="25"/>
+      <c r="C154" s="12"/>
+      <c r="D154" s="12"/>
+      <c r="E154" s="12"/>
+      <c r="F154" s="12"/>
+      <c r="G154" s="13"/>
     </row>
     <row r="155" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B155" s="1" t="s">
@@ -3046,8 +3068,12 @@
       <c r="E156" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F156" s="4"/>
-      <c r="G156" s="5"/>
+      <c r="F156" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G156" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="157" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B157" s="3">
@@ -3060,8 +3086,12 @@
       <c r="E157" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F157" s="4"/>
-      <c r="G157" s="5"/>
+      <c r="F157" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G157" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="158" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B158" s="3">
@@ -3074,8 +3104,12 @@
       <c r="E158" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F158" s="4"/>
-      <c r="G158" s="5"/>
+      <c r="F158" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G158" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="159" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B159" s="3">
@@ -3088,8 +3122,12 @@
       <c r="E159" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F159" s="4"/>
-      <c r="G159" s="5"/>
+      <c r="F159" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G159" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="160" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B160" s="3">
@@ -3102,8 +3140,12 @@
       <c r="E160" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F160" s="4"/>
-      <c r="G160" s="5"/>
+      <c r="F160" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G160" s="31" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="161" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B161" s="8" t="s">
@@ -3120,6 +3162,179 @@
     <row r="162" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="197">
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="D151:G151"/>
+    <mergeCell ref="B152:C153"/>
+    <mergeCell ref="D152:G152"/>
+    <mergeCell ref="D153:G153"/>
+    <mergeCell ref="B154:G154"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="D137:G137"/>
+    <mergeCell ref="B138:C139"/>
+    <mergeCell ref="D138:G138"/>
+    <mergeCell ref="D139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="B123:G123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:G134"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="D136:G136"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="B121:C122"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="D122:G122"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:G108"/>
+    <mergeCell ref="B109:C110"/>
+    <mergeCell ref="D109:G109"/>
+    <mergeCell ref="D110:G110"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:G107"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B17:C19"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B71:C72"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:G83"/>
     <mergeCell ref="C104:D104"/>
     <mergeCell ref="B105:C105"/>
     <mergeCell ref="D105:G105"/>
@@ -3144,179 +3359,6 @@
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B71:C72"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="D107:G107"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:G108"/>
-    <mergeCell ref="B109:C110"/>
-    <mergeCell ref="D109:G109"/>
-    <mergeCell ref="D110:G110"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:G117"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="B121:C122"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="D122:G122"/>
-    <mergeCell ref="B123:G123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:G134"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="D136:G136"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="D137:G137"/>
-    <mergeCell ref="B138:C139"/>
-    <mergeCell ref="D138:G138"/>
-    <mergeCell ref="D139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="D151:G151"/>
-    <mergeCell ref="B152:C153"/>
-    <mergeCell ref="D152:G152"/>
-    <mergeCell ref="D153:G153"/>
-    <mergeCell ref="B154:G154"/>
-    <mergeCell ref="C155:D155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Partial commit with the 2 test cases for selenium
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D2FB28-7EA7-4D61-9486-B7AC1EF893FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF5BDA4-1E5A-4EA9-8F2E-41EC68846022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="160">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -781,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -796,7 +796,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -811,15 +811,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -858,6 +849,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,9 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1159,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1175,10 +1172,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="6">
         <v>1</v>
       </c>
@@ -1187,10 +1184,10 @@
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1199,36 +1196,36 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
     </row>
     <row r="7" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
@@ -1332,10 +1329,10 @@
     </row>
     <row r="14" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="15" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="6">
         <v>2</v>
       </c>
@@ -1344,10 +1341,10 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="6" t="s">
         <v>93</v>
       </c>
@@ -1356,26 +1353,26 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20" t="s">
+      <c r="C17" s="14"/>
+      <c r="D17" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="22"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="23" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="26"/>
@@ -1388,14 +1385,14 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="25"/>
     </row>
     <row r="21" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="1" t="s">
@@ -1499,10 +1496,10 @@
     </row>
     <row r="28" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="29" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="6">
         <v>3</v>
       </c>
@@ -1511,10 +1508,10 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="6" t="s">
         <v>94</v>
       </c>
@@ -1523,36 +1520,36 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="17"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="14"/>
+      <c r="D31" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="22"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
     </row>
     <row r="32" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="23" t="s">
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="1" t="s">
@@ -1670,10 +1667,10 @@
     </row>
     <row r="42" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="43" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C43" s="15"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="6">
         <v>4</v>
       </c>
@@ -1682,10 +1679,10 @@
       <c r="G43" s="7"/>
     </row>
     <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="6" t="s">
         <v>95</v>
       </c>
@@ -1694,36 +1691,36 @@
       <c r="G44" s="7"/>
     </row>
     <row r="45" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="20" t="s">
+      <c r="C45" s="14"/>
+      <c r="D45" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="23" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="25"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="13"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="25"/>
     </row>
     <row r="48" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B48" s="1" t="s">
@@ -1827,10 +1824,10 @@
     </row>
     <row r="55" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="56" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C56" s="15"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="6">
         <v>5</v>
       </c>
@@ -1839,10 +1836,10 @@
       <c r="G56" s="7"/>
     </row>
     <row r="57" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C57" s="15"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="6" t="s">
         <v>51</v>
       </c>
@@ -1851,36 +1848,36 @@
       <c r="G57" s="7"/>
     </row>
     <row r="58" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="17"/>
-      <c r="D58" s="20" t="s">
+      <c r="C58" s="14"/>
+      <c r="D58" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="22"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="23" t="s">
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="25"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="22"/>
     </row>
     <row r="60" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="13"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="25"/>
     </row>
     <row r="61" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B61" s="1" t="s">
@@ -1984,10 +1981,10 @@
     </row>
     <row r="68" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="69" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="15"/>
+      <c r="C69" s="12"/>
       <c r="D69" s="6">
         <v>6</v>
       </c>
@@ -1996,10 +1993,10 @@
       <c r="G69" s="7"/>
     </row>
     <row r="70" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="15"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="6" t="s">
         <v>79</v>
       </c>
@@ -2008,36 +2005,36 @@
       <c r="G70" s="7"/>
     </row>
     <row r="71" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="20" t="s">
+      <c r="C71" s="14"/>
+      <c r="D71" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="22"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="19"/>
     </row>
     <row r="72" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B72" s="18"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="23" t="s">
+      <c r="B72" s="15"/>
+      <c r="C72" s="16"/>
+      <c r="D72" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="25"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="22"/>
     </row>
     <row r="73" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="13"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="25"/>
     </row>
     <row r="74" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B74" s="1" t="s">
@@ -2155,10 +2152,10 @@
     </row>
     <row r="82" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="83" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="15"/>
+      <c r="C83" s="12"/>
       <c r="D83" s="6">
         <v>7</v>
       </c>
@@ -2167,10 +2164,10 @@
       <c r="G83" s="7"/>
     </row>
     <row r="84" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="15"/>
+      <c r="C84" s="12"/>
       <c r="D84" s="6" t="s">
         <v>66</v>
       </c>
@@ -2179,36 +2176,36 @@
       <c r="G84" s="7"/>
     </row>
     <row r="85" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="17"/>
-      <c r="D85" s="20" t="s">
+      <c r="C85" s="14"/>
+      <c r="D85" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="22"/>
+      <c r="E85" s="18"/>
+      <c r="F85" s="18"/>
+      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="23" t="s">
+      <c r="B86" s="15"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="25"/>
+      <c r="E86" s="21"/>
+      <c r="F86" s="21"/>
+      <c r="G86" s="22"/>
     </row>
     <row r="87" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="12"/>
-      <c r="G87" s="13"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="25"/>
     </row>
     <row r="88" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B88" s="1" t="s">
@@ -2298,10 +2295,10 @@
     </row>
     <row r="94" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="95" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C95" s="15"/>
+      <c r="C95" s="12"/>
       <c r="D95" s="6">
         <v>8</v>
       </c>
@@ -2310,10 +2307,10 @@
       <c r="G95" s="7"/>
     </row>
     <row r="96" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="15"/>
+      <c r="C96" s="12"/>
       <c r="D96" s="6" t="s">
         <v>96</v>
       </c>
@@ -2322,36 +2319,36 @@
       <c r="G96" s="7"/>
     </row>
     <row r="97" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C97" s="17"/>
-      <c r="D97" s="20" t="s">
+      <c r="C97" s="14"/>
+      <c r="D97" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
-      <c r="G97" s="22"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="19"/>
     </row>
     <row r="98" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B98" s="18"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="23" t="s">
+      <c r="B98" s="15"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="25"/>
+      <c r="E98" s="21"/>
+      <c r="F98" s="21"/>
+      <c r="G98" s="22"/>
     </row>
     <row r="99" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C99" s="12"/>
-      <c r="D99" s="12"/>
-      <c r="E99" s="12"/>
-      <c r="F99" s="12"/>
-      <c r="G99" s="13"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="25"/>
     </row>
     <row r="100" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B100" s="1" t="s">
@@ -2441,10 +2438,10 @@
     </row>
     <row r="106" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="107" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C107" s="15"/>
+      <c r="C107" s="12"/>
       <c r="D107" s="6">
         <v>9</v>
       </c>
@@ -2453,10 +2450,10 @@
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C108" s="15"/>
+      <c r="C108" s="12"/>
       <c r="D108" s="6" t="s">
         <v>106</v>
       </c>
@@ -2465,36 +2462,36 @@
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C109" s="17"/>
-      <c r="D109" s="20" t="s">
+      <c r="C109" s="14"/>
+      <c r="D109" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E109" s="21"/>
-      <c r="F109" s="21"/>
-      <c r="G109" s="22"/>
+      <c r="E109" s="18"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="19"/>
     </row>
     <row r="110" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B110" s="18"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="23" t="s">
+      <c r="B110" s="15"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E110" s="24"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="25"/>
+      <c r="E110" s="21"/>
+      <c r="F110" s="21"/>
+      <c r="G110" s="22"/>
     </row>
     <row r="111" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B111" s="11" t="s">
+      <c r="B111" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C111" s="12"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="12"/>
-      <c r="F111" s="12"/>
-      <c r="G111" s="13"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="25"/>
     </row>
     <row r="112" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B112" s="1" t="s">
@@ -2528,7 +2525,7 @@
       <c r="F113" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G113" s="31" t="s">
+      <c r="G113" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2546,7 +2543,7 @@
       <c r="F114" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G114" s="31" t="s">
+      <c r="G114" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2564,7 +2561,7 @@
       <c r="F115" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G115" s="31" t="s">
+      <c r="G115" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2582,7 +2579,7 @@
       <c r="F116" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G116" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2600,10 +2597,10 @@
     </row>
     <row r="118" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="119" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="15"/>
+      <c r="C119" s="12"/>
       <c r="D119" s="6">
         <v>10</v>
       </c>
@@ -2612,10 +2609,10 @@
       <c r="G119" s="7"/>
     </row>
     <row r="120" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C120" s="15"/>
+      <c r="C120" s="12"/>
       <c r="D120" s="6" t="s">
         <v>117</v>
       </c>
@@ -2624,36 +2621,36 @@
       <c r="G120" s="7"/>
     </row>
     <row r="121" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C121" s="17"/>
-      <c r="D121" s="20" t="s">
+      <c r="C121" s="14"/>
+      <c r="D121" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
-      <c r="G121" s="22"/>
+      <c r="E121" s="18"/>
+      <c r="F121" s="18"/>
+      <c r="G121" s="19"/>
     </row>
     <row r="122" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B122" s="18"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="23" t="s">
+      <c r="B122" s="15"/>
+      <c r="C122" s="16"/>
+      <c r="D122" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E122" s="24"/>
-      <c r="F122" s="24"/>
-      <c r="G122" s="25"/>
+      <c r="E122" s="21"/>
+      <c r="F122" s="21"/>
+      <c r="G122" s="22"/>
     </row>
     <row r="123" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C123" s="12"/>
-      <c r="D123" s="12"/>
-      <c r="E123" s="12"/>
-      <c r="F123" s="12"/>
-      <c r="G123" s="13"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="25"/>
     </row>
     <row r="124" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B124" s="1" t="s">
@@ -2684,8 +2681,12 @@
       <c r="E125" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F125" s="4"/>
-      <c r="G125" s="5"/>
+      <c r="F125" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G125" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="126" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B126" s="3">
@@ -2698,8 +2699,12 @@
       <c r="E126" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F126" s="4"/>
-      <c r="G126" s="5"/>
+      <c r="F126" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G126" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="127" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B127" s="3">
@@ -2712,8 +2717,12 @@
       <c r="E127" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F127" s="4"/>
-      <c r="G127" s="5"/>
+      <c r="F127" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="G127" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="128" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B128" s="3">
@@ -2726,8 +2735,12 @@
       <c r="E128" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F128" s="4"/>
-      <c r="G128" s="5"/>
+      <c r="F128" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G128" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="129" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B129" s="3">
@@ -2740,8 +2753,12 @@
       <c r="E129" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F129" s="4"/>
-      <c r="G129" s="5"/>
+      <c r="F129" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G129" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="130" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B130" s="3">
@@ -2754,8 +2771,12 @@
       <c r="E130" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F130" s="4"/>
-      <c r="G130" s="5"/>
+      <c r="F130" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="131" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B131" s="3">
@@ -2768,8 +2789,12 @@
       <c r="E131" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F131" s="4"/>
-      <c r="G131" s="5"/>
+      <c r="F131" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G131" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="132" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B132" s="3">
@@ -2782,8 +2807,12 @@
       <c r="E132" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F132" s="4"/>
-      <c r="G132" s="5"/>
+      <c r="F132" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G132" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="133" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B133" s="3">
@@ -2796,8 +2825,12 @@
       <c r="E133" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F133" s="4"/>
-      <c r="G133" s="5"/>
+      <c r="F133" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G133" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="134" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B134" s="8" t="s">
@@ -2813,10 +2846,10 @@
     </row>
     <row r="135" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="136" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B136" s="14" t="s">
+      <c r="B136" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C136" s="15"/>
+      <c r="C136" s="12"/>
       <c r="D136" s="6">
         <v>11</v>
       </c>
@@ -2825,10 +2858,10 @@
       <c r="G136" s="7"/>
     </row>
     <row r="137" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B137" s="14" t="s">
+      <c r="B137" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C137" s="15"/>
+      <c r="C137" s="12"/>
       <c r="D137" s="6" t="s">
         <v>147</v>
       </c>
@@ -2837,36 +2870,36 @@
       <c r="G137" s="7"/>
     </row>
     <row r="138" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B138" s="16" t="s">
+      <c r="B138" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C138" s="17"/>
-      <c r="D138" s="20" t="s">
+      <c r="C138" s="14"/>
+      <c r="D138" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E138" s="21"/>
-      <c r="F138" s="21"/>
-      <c r="G138" s="22"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="18"/>
+      <c r="G138" s="19"/>
     </row>
     <row r="139" spans="2:7" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B139" s="18"/>
-      <c r="C139" s="19"/>
-      <c r="D139" s="23" t="s">
+      <c r="B139" s="15"/>
+      <c r="C139" s="16"/>
+      <c r="D139" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E139" s="24"/>
-      <c r="F139" s="24"/>
-      <c r="G139" s="25"/>
+      <c r="E139" s="21"/>
+      <c r="F139" s="21"/>
+      <c r="G139" s="22"/>
     </row>
     <row r="140" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B140" s="11" t="s">
+      <c r="B140" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C140" s="12"/>
-      <c r="D140" s="12"/>
-      <c r="E140" s="12"/>
-      <c r="F140" s="12"/>
-      <c r="G140" s="13"/>
+      <c r="C140" s="24"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="24"/>
+      <c r="G140" s="25"/>
     </row>
     <row r="141" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B141" s="1" t="s">
@@ -2897,8 +2930,12 @@
       <c r="E142" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F142" s="4"/>
-      <c r="G142" s="5"/>
+      <c r="F142" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G142" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="143" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B143" s="3">
@@ -2911,8 +2948,12 @@
       <c r="E143" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F143" s="4"/>
-      <c r="G143" s="5"/>
+      <c r="F143" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G143" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="144" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B144" s="3">
@@ -2925,8 +2966,12 @@
       <c r="E144" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F144" s="4"/>
-      <c r="G144" s="5"/>
+      <c r="F144" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G144" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="145" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B145" s="3">
@@ -2939,8 +2984,12 @@
       <c r="E145" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F145" s="4"/>
-      <c r="G145" s="5"/>
+      <c r="F145" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G145" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="146" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B146" s="3">
@@ -2953,8 +3002,12 @@
       <c r="E146" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F146" s="4"/>
-      <c r="G146" s="5"/>
+      <c r="F146" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G146" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="147" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B147" s="3">
@@ -2967,8 +3020,12 @@
       <c r="E147" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="F147" s="4"/>
-      <c r="G147" s="5"/>
+      <c r="F147" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G147" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="148" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B148" s="8" t="s">
@@ -2984,10 +3041,10 @@
     </row>
     <row r="149" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="150" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B150" s="14" t="s">
+      <c r="B150" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C150" s="15"/>
+      <c r="C150" s="12"/>
       <c r="D150" s="6">
         <v>12</v>
       </c>
@@ -2996,10 +3053,10 @@
       <c r="G150" s="7"/>
     </row>
     <row r="151" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B151" s="14" t="s">
+      <c r="B151" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C151" s="15"/>
+      <c r="C151" s="12"/>
       <c r="D151" s="6" t="s">
         <v>137</v>
       </c>
@@ -3008,36 +3065,36 @@
       <c r="G151" s="7"/>
     </row>
     <row r="152" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B152" s="16" t="s">
+      <c r="B152" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C152" s="17"/>
-      <c r="D152" s="20" t="s">
+      <c r="C152" s="14"/>
+      <c r="D152" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E152" s="21"/>
-      <c r="F152" s="21"/>
-      <c r="G152" s="22"/>
+      <c r="E152" s="18"/>
+      <c r="F152" s="18"/>
+      <c r="G152" s="19"/>
     </row>
     <row r="153" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B153" s="18"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="23" t="s">
+      <c r="B153" s="15"/>
+      <c r="C153" s="16"/>
+      <c r="D153" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E153" s="24"/>
-      <c r="F153" s="24"/>
-      <c r="G153" s="25"/>
+      <c r="E153" s="21"/>
+      <c r="F153" s="21"/>
+      <c r="G153" s="22"/>
     </row>
     <row r="154" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C154" s="12"/>
-      <c r="D154" s="12"/>
-      <c r="E154" s="12"/>
-      <c r="F154" s="12"/>
-      <c r="G154" s="13"/>
+      <c r="C154" s="24"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="24"/>
+      <c r="F154" s="24"/>
+      <c r="G154" s="25"/>
     </row>
     <row r="155" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B155" s="1" t="s">
@@ -3071,7 +3128,7 @@
       <c r="F156" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G156" s="31" t="s">
+      <c r="G156" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3089,7 +3146,7 @@
       <c r="F157" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="G157" s="31" t="s">
+      <c r="G157" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3107,7 +3164,7 @@
       <c r="F158" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G158" s="31" t="s">
+      <c r="G158" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3125,7 +3182,7 @@
       <c r="F159" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G159" s="31" t="s">
+      <c r="G159" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3143,7 +3200,7 @@
       <c r="F160" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="G160" s="31" t="s">
+      <c r="G160" s="5" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3162,72 +3219,113 @@
     <row r="162" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="197">
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="C159:D159"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="B151:C151"/>
-    <mergeCell ref="D151:G151"/>
-    <mergeCell ref="B152:C153"/>
-    <mergeCell ref="D152:G152"/>
-    <mergeCell ref="D153:G153"/>
-    <mergeCell ref="B154:G154"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="D137:G137"/>
-    <mergeCell ref="B138:C139"/>
-    <mergeCell ref="D138:G138"/>
-    <mergeCell ref="D139:G139"/>
-    <mergeCell ref="B140:G140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="B123:G123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="B134:C134"/>
-    <mergeCell ref="D134:G134"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="D136:G136"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:G117"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="B121:C122"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="D122:G122"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="D108:G108"/>
-    <mergeCell ref="B109:C110"/>
-    <mergeCell ref="D109:G109"/>
-    <mergeCell ref="D110:G110"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D105:G105"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="B99:G99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="B97:C98"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="D98:G98"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="D93:G93"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:G95"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="B85:C86"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:G81"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B71:C72"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="D59:G59"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:G54"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B17:C19"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="B3:C3"/>
@@ -3252,113 +3350,72 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B17:C19"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="B31:C32"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:G27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:G41"/>
-    <mergeCell ref="B33:G33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:G43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="D45:G45"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:G57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:G54"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:G67"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:G69"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B71:C72"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:G84"/>
-    <mergeCell ref="B85:C86"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:G81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:G83"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D105:G105"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="B99:G99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:G96"/>
-    <mergeCell ref="B97:C98"/>
-    <mergeCell ref="D97:G97"/>
-    <mergeCell ref="D98:G98"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="D93:G93"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:G95"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="D108:G108"/>
+    <mergeCell ref="B109:C110"/>
+    <mergeCell ref="D109:G109"/>
+    <mergeCell ref="D110:G110"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:G117"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="B121:C122"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="D122:G122"/>
+    <mergeCell ref="B123:G123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:G134"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="D136:G136"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="D137:G137"/>
+    <mergeCell ref="B138:C139"/>
+    <mergeCell ref="D138:G138"/>
+    <mergeCell ref="D139:G139"/>
+    <mergeCell ref="B140:G140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="C159:D159"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="B151:C151"/>
+    <mergeCell ref="D151:G151"/>
+    <mergeCell ref="B152:C153"/>
+    <mergeCell ref="D152:G152"/>
+    <mergeCell ref="D153:G153"/>
+    <mergeCell ref="B154:G154"/>
+    <mergeCell ref="C155:D155"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the 2 test cases that were implemented in jmeter
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roxy Enescu\Desktop\SoftwareApplicationTesting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB3737B-F079-4528-BB06-E71D696A2641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEF6D63-E1CB-4D4F-AC54-398D3F4B3978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testarea funcțională" sheetId="1" r:id="rId1"/>
+    <sheet name="Testarea de performanță" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="188">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -520,6 +521,75 @@
   </si>
   <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>Maxi Pet - Adăugare produs de la promoții în coș</t>
+  </si>
+  <si>
+    <t>Se navighează spre pagina "Promoții"</t>
+  </si>
+  <si>
+    <t>Se afișează pagina unde sunt listate produsele la promoție</t>
+  </si>
+  <si>
+    <t>Se selectează produsul "GOURMET Gold Pachet conserve Mousse cu Vită, Ton, Ficat şi Curcan 4x85g"</t>
+  </si>
+  <si>
+    <t>Se vizualizează pagina produsului selectat</t>
+  </si>
+  <si>
+    <t>Se apasă butonul "ADAUGĂ ÎN COȘ"</t>
+  </si>
+  <si>
+    <t>Produsul selectat este adăugat în coș</t>
+  </si>
+  <si>
+    <t>Se apasă pe iconița ce reprezintă coșul de cumpărături</t>
+  </si>
+  <si>
+    <t>Se afișează o fereastră cu coșul</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul "Continuă cumpărăturile"</t>
+  </si>
+  <si>
+    <t>Se vizualizează coșul de cumpărături</t>
+  </si>
+  <si>
+    <t>Coșul de cumpărături este actualizat și conține produsul adăugat</t>
+  </si>
+  <si>
+    <t>Maxi Pet - Vizualizare produs după căutare</t>
+  </si>
+  <si>
+    <t>Se apasă pe bara de căutare</t>
+  </si>
+  <si>
+    <t>Se afișează bara de căutare extinsă</t>
+  </si>
+  <si>
+    <t>Se introduce textul "jucarie"</t>
+  </si>
+  <si>
+    <t>Textul din bara de căutare se actualizează</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul cu lupă</t>
+  </si>
+  <si>
+    <t>Se afișează pagina cu toate jucăriile</t>
+  </si>
+  <si>
+    <t>Se redirecționează către pagina de căutare</t>
+  </si>
+  <si>
+    <t>Se selectează produsul "CROCI Jucărie pentru pisici, Croissant din pluş cu iarba pisicii"</t>
+  </si>
+  <si>
+    <t>Se afișează pagina jucăriei</t>
+  </si>
+  <si>
+    <t>Se poate vizualiza pagina jucăriei selectate</t>
   </si>
 </sst>
 </file>
@@ -849,15 +919,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -892,6 +953,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1192,26 +1262,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56:D56"/>
+    <sheetView topLeftCell="A149" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B154" sqref="B154:G165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" customWidth="1"/>
-    <col min="6" max="6" width="29.77734375" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" customWidth="1"/>
+    <col min="4" max="4" width="33.86328125" customWidth="1"/>
+    <col min="5" max="5" width="22.19921875" customWidth="1"/>
+    <col min="6" max="6" width="29.796875" customWidth="1"/>
+    <col min="7" max="7" width="19.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="9">
         <v>1</v>
       </c>
@@ -1219,11 +1289,11 @@
       <c r="F2" s="13"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1231,39 +1301,39 @@
       <c r="F3" s="13"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="23" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="26" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="22"/>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1281,7 +1351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1295,7 +1365,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="3">
         <v>2</v>
       </c>
@@ -1309,7 +1379,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="3">
         <v>3</v>
       </c>
@@ -1323,7 +1393,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="3">
         <v>4</v>
       </c>
@@ -1337,7 +1407,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="3">
         <v>5</v>
       </c>
@@ -1351,7 +1421,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="3">
         <v>6</v>
       </c>
@@ -1365,7 +1435,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
@@ -1377,12 +1447,12 @@
       <c r="F14" s="13"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="17" t="s">
+    <row r="15" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="9">
         <v>2</v>
       </c>
@@ -1390,11 +1460,11 @@
       <c r="F16" s="13"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="17" t="s">
+    <row r="17" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="9" t="s">
         <v>90</v>
       </c>
@@ -1402,29 +1472,29 @@
       <c r="F17" s="13"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="19" t="s">
+    <row r="18" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="23" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="26" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B20" s="29"/>
       <c r="C20" s="30"/>
       <c r="D20" s="31" t="s">
@@ -1434,17 +1504,17 @@
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
     </row>
-    <row r="21" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="14" t="s">
+    <row r="21" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1532,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="3">
         <v>1</v>
       </c>
@@ -1476,7 +1546,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="3">
         <v>2</v>
       </c>
@@ -1490,7 +1560,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="3">
         <v>3</v>
       </c>
@@ -1504,7 +1574,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B26" s="3">
         <v>4</v>
       </c>
@@ -1518,7 +1588,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="3">
         <v>5</v>
       </c>
@@ -1532,7 +1602,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B28" s="3">
         <v>6</v>
       </c>
@@ -1546,7 +1616,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B29" s="11" t="s">
         <v>8</v>
       </c>
@@ -1558,12 +1628,12 @@
       <c r="F29" s="13"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="17" t="s">
+    <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="31" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B31" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="18"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="9">
         <v>3</v>
       </c>
@@ -1571,11 +1641,11 @@
       <c r="F31" s="13"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="17" t="s">
+    <row r="32" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="15"/>
       <c r="D32" s="9" t="s">
         <v>91</v>
       </c>
@@ -1583,39 +1653,39 @@
       <c r="F32" s="13"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="19" t="s">
+    <row r="33" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="23" t="s">
+      <c r="C33" s="17"/>
+      <c r="D33" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="25"/>
-    </row>
-    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="26" t="s">
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
+    </row>
+    <row r="34" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="18"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-    </row>
-    <row r="35" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="14" t="s">
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
@@ -1633,7 +1703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B37" s="3">
         <v>1</v>
       </c>
@@ -1651,7 +1721,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B38" s="3">
         <v>2</v>
       </c>
@@ -1669,7 +1739,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B39" s="3">
         <v>3</v>
       </c>
@@ -1687,7 +1757,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B40" s="3">
         <v>4</v>
       </c>
@@ -1705,7 +1775,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B41" s="3">
         <v>5</v>
       </c>
@@ -1723,7 +1793,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B42" s="3">
         <v>6</v>
       </c>
@@ -1741,7 +1811,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B43" s="3">
         <v>7</v>
       </c>
@@ -1759,7 +1829,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B44" s="11" t="s">
         <v>8</v>
       </c>
@@ -1771,12 +1841,12 @@
       <c r="F44" s="13"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="17" t="s">
+    <row r="45" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B46" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="18"/>
+      <c r="C46" s="15"/>
       <c r="D46" s="9">
         <v>4</v>
       </c>
@@ -1784,11 +1854,11 @@
       <c r="F46" s="13"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="17" t="s">
+    <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B47" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="15"/>
       <c r="D47" s="9" t="s">
         <v>92</v>
       </c>
@@ -1796,39 +1866,39 @@
       <c r="F47" s="13"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="19" t="s">
+    <row r="48" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="23" t="s">
+      <c r="C48" s="17"/>
+      <c r="D48" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="25"/>
-    </row>
-    <row r="49" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="26" t="s">
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="22"/>
+    </row>
+    <row r="49" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="28"/>
-    </row>
-    <row r="50" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="14" t="s">
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="25"/>
+    </row>
+    <row r="50" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B50" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
-    </row>
-    <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B52" s="3">
         <v>1</v>
       </c>
@@ -1864,7 +1934,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B53" s="3">
         <v>2</v>
       </c>
@@ -1882,7 +1952,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B54" s="3">
         <v>3</v>
       </c>
@@ -1900,7 +1970,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B55" s="3">
         <v>4</v>
       </c>
@@ -1918,7 +1988,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B56" s="3">
         <v>5</v>
       </c>
@@ -1936,7 +2006,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B57" s="3">
         <v>6</v>
       </c>
@@ -1954,7 +2024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B58" s="11" t="s">
         <v>8</v>
       </c>
@@ -1966,12 +2036,12 @@
       <c r="F58" s="13"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="17" t="s">
+    <row r="59" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="60" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B60" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="18"/>
+      <c r="C60" s="15"/>
       <c r="D60" s="9">
         <v>5</v>
       </c>
@@ -1979,11 +2049,11 @@
       <c r="F60" s="13"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="17" t="s">
+    <row r="61" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B61" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="18"/>
+      <c r="C61" s="15"/>
       <c r="D61" s="9" t="s">
         <v>48</v>
       </c>
@@ -1991,39 +2061,39 @@
       <c r="F61" s="13"/>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="19" t="s">
+    <row r="62" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="23" t="s">
+      <c r="C62" s="17"/>
+      <c r="D62" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="25"/>
-    </row>
-    <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="21"/>
-      <c r="C63" s="22"/>
-      <c r="D63" s="26" t="s">
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="22"/>
+    </row>
+    <row r="63" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="27"/>
-      <c r="F63" s="27"/>
-      <c r="G63" s="28"/>
-    </row>
-    <row r="64" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="14" t="s">
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="25"/>
+    </row>
+    <row r="64" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B64" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="16"/>
-    </row>
-    <row r="65" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="28"/>
+    </row>
+    <row r="65" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B66" s="3">
         <v>1</v>
       </c>
@@ -2055,7 +2125,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B67" s="3">
         <v>2</v>
       </c>
@@ -2069,7 +2139,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B68" s="3">
         <v>3</v>
       </c>
@@ -2083,7 +2153,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B69" s="3">
         <v>4</v>
       </c>
@@ -2097,7 +2167,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B70" s="3">
         <v>5</v>
       </c>
@@ -2111,7 +2181,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="5"/>
     </row>
-    <row r="71" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B71" s="11" t="s">
         <v>8</v>
       </c>
@@ -2123,12 +2193,12 @@
       <c r="F71" s="13"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="73" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="17" t="s">
+    <row r="72" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="73" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B73" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="18"/>
+      <c r="C73" s="15"/>
       <c r="D73" s="9">
         <v>6</v>
       </c>
@@ -2136,11 +2206,11 @@
       <c r="F73" s="13"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="17" t="s">
+    <row r="74" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B74" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="18"/>
+      <c r="C74" s="15"/>
       <c r="D74" s="9" t="s">
         <v>76</v>
       </c>
@@ -2148,39 +2218,39 @@
       <c r="F74" s="13"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="19" t="s">
+    <row r="75" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B75" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="23" t="s">
+      <c r="C75" s="17"/>
+      <c r="D75" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
-    </row>
-    <row r="76" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="21"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="26" t="s">
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="22"/>
+    </row>
+    <row r="76" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B76" s="18"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="27"/>
-      <c r="G76" s="28"/>
-    </row>
-    <row r="77" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="14" t="s">
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="25"/>
+    </row>
+    <row r="77" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B77" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C77" s="15"/>
-      <c r="D77" s="15"/>
-      <c r="E77" s="15"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
-    </row>
-    <row r="78" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C77" s="27"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="27"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="28"/>
+    </row>
+    <row r="78" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
@@ -2198,7 +2268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B79" s="3">
         <v>1</v>
       </c>
@@ -2212,7 +2282,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B80" s="3">
         <v>2</v>
       </c>
@@ -2226,7 +2296,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B81" s="3">
         <v>3</v>
       </c>
@@ -2240,7 +2310,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B82" s="3">
         <v>4</v>
       </c>
@@ -2254,7 +2324,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B83" s="3">
         <v>4</v>
       </c>
@@ -2268,7 +2338,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B84" s="3">
         <v>5</v>
       </c>
@@ -2282,7 +2352,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B85" s="11" t="s">
         <v>8</v>
       </c>
@@ -2294,12 +2364,12 @@
       <c r="F85" s="13"/>
       <c r="G85" s="10"/>
     </row>
-    <row r="86" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="17" t="s">
+    <row r="86" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="87" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B87" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C87" s="18"/>
+      <c r="C87" s="15"/>
       <c r="D87" s="9">
         <v>7</v>
       </c>
@@ -2307,11 +2377,11 @@
       <c r="F87" s="13"/>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="17" t="s">
+    <row r="88" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B88" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="18"/>
+      <c r="C88" s="15"/>
       <c r="D88" s="9" t="s">
         <v>63</v>
       </c>
@@ -2319,39 +2389,39 @@
       <c r="F88" s="13"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="19" t="s">
+    <row r="89" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B89" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C89" s="20"/>
-      <c r="D89" s="23" t="s">
+      <c r="C89" s="17"/>
+      <c r="D89" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E89" s="24"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="25"/>
-    </row>
-    <row r="90" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B90" s="21"/>
-      <c r="C90" s="22"/>
-      <c r="D90" s="26" t="s">
+      <c r="E89" s="21"/>
+      <c r="F89" s="21"/>
+      <c r="G89" s="22"/>
+    </row>
+    <row r="90" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B90" s="18"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E90" s="27"/>
-      <c r="F90" s="27"/>
-      <c r="G90" s="28"/>
-    </row>
-    <row r="91" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="14" t="s">
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
+    </row>
+    <row r="91" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B91" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C91" s="15"/>
-      <c r="D91" s="15"/>
-      <c r="E91" s="15"/>
-      <c r="F91" s="15"/>
-      <c r="G91" s="16"/>
-    </row>
-    <row r="92" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C91" s="27"/>
+      <c r="D91" s="27"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="28"/>
+    </row>
+    <row r="92" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B92" s="1" t="s">
         <v>3</v>
       </c>
@@ -2369,7 +2439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B93" s="3">
         <v>1</v>
       </c>
@@ -2383,7 +2453,7 @@
       <c r="F93" s="4"/>
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B94" s="3">
         <v>2</v>
       </c>
@@ -2397,7 +2467,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B95" s="3">
         <v>3</v>
       </c>
@@ -2411,7 +2481,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B96" s="3">
         <v>4</v>
       </c>
@@ -2425,7 +2495,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B97" s="11" t="s">
         <v>8</v>
       </c>
@@ -2437,12 +2507,12 @@
       <c r="F97" s="13"/>
       <c r="G97" s="10"/>
     </row>
-    <row r="98" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="99" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B99" s="17" t="s">
+    <row r="98" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="99" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B99" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C99" s="18"/>
+      <c r="C99" s="15"/>
       <c r="D99" s="9">
         <v>8</v>
       </c>
@@ -2450,11 +2520,11 @@
       <c r="F99" s="13"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B100" s="17" t="s">
+    <row r="100" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B100" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C100" s="18"/>
+      <c r="C100" s="15"/>
       <c r="D100" s="9" t="s">
         <v>93</v>
       </c>
@@ -2462,39 +2532,39 @@
       <c r="F100" s="13"/>
       <c r="G100" s="10"/>
     </row>
-    <row r="101" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="19" t="s">
+    <row r="101" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B101" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C101" s="20"/>
-      <c r="D101" s="23" t="s">
+      <c r="C101" s="17"/>
+      <c r="D101" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="25"/>
-    </row>
-    <row r="102" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B102" s="21"/>
-      <c r="C102" s="22"/>
-      <c r="D102" s="26" t="s">
+      <c r="E101" s="21"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="22"/>
+    </row>
+    <row r="102" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B102" s="18"/>
+      <c r="C102" s="19"/>
+      <c r="D102" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="28"/>
-    </row>
-    <row r="103" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="14" t="s">
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="25"/>
+    </row>
+    <row r="103" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B103" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="16"/>
-    </row>
-    <row r="104" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
+      <c r="G103" s="28"/>
+    </row>
+    <row r="104" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B104" s="1" t="s">
         <v>3</v>
       </c>
@@ -2512,7 +2582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B105" s="3">
         <v>1</v>
       </c>
@@ -2526,7 +2596,7 @@
       <c r="F105" s="4"/>
       <c r="G105" s="5"/>
     </row>
-    <row r="106" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B106" s="3">
         <v>2</v>
       </c>
@@ -2540,7 +2610,7 @@
       <c r="F106" s="4"/>
       <c r="G106" s="5"/>
     </row>
-    <row r="107" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B107" s="3">
         <v>3</v>
       </c>
@@ -2554,7 +2624,7 @@
       <c r="F107" s="4"/>
       <c r="G107" s="5"/>
     </row>
-    <row r="108" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B108" s="3">
         <v>4</v>
       </c>
@@ -2568,7 +2638,7 @@
       <c r="F108" s="4"/>
       <c r="G108" s="5"/>
     </row>
-    <row r="109" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B109" s="11" t="s">
         <v>8</v>
       </c>
@@ -2580,12 +2650,12 @@
       <c r="F109" s="13"/>
       <c r="G109" s="10"/>
     </row>
-    <row r="110" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="111" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B111" s="17" t="s">
+    <row r="110" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="111" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B111" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C111" s="18"/>
+      <c r="C111" s="15"/>
       <c r="D111" s="9">
         <v>9</v>
       </c>
@@ -2593,11 +2663,11 @@
       <c r="F111" s="13"/>
       <c r="G111" s="10"/>
     </row>
-    <row r="112" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B112" s="17" t="s">
+    <row r="112" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B112" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C112" s="18"/>
+      <c r="C112" s="15"/>
       <c r="D112" s="9" t="s">
         <v>103</v>
       </c>
@@ -2605,39 +2675,39 @@
       <c r="F112" s="13"/>
       <c r="G112" s="10"/>
     </row>
-    <row r="113" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="19" t="s">
+    <row r="113" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B113" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="20"/>
-      <c r="D113" s="23" t="s">
+      <c r="C113" s="17"/>
+      <c r="D113" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E113" s="24"/>
-      <c r="F113" s="24"/>
-      <c r="G113" s="25"/>
-    </row>
-    <row r="114" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B114" s="21"/>
-      <c r="C114" s="22"/>
-      <c r="D114" s="26" t="s">
+      <c r="E113" s="21"/>
+      <c r="F113" s="21"/>
+      <c r="G113" s="22"/>
+    </row>
+    <row r="114" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B114" s="18"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="28"/>
-    </row>
-    <row r="115" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B115" s="14" t="s">
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="25"/>
+    </row>
+    <row r="115" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B115" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C115" s="15"/>
-      <c r="D115" s="15"/>
-      <c r="E115" s="15"/>
-      <c r="F115" s="15"/>
-      <c r="G115" s="16"/>
-    </row>
-    <row r="116" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="28"/>
+    </row>
+    <row r="116" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B116" s="1" t="s">
         <v>3</v>
       </c>
@@ -2655,7 +2725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B117" s="3">
         <v>1</v>
       </c>
@@ -2673,7 +2743,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="118" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B118" s="3">
         <v>2</v>
       </c>
@@ -2691,7 +2761,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7" ht="44" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B119" s="3">
         <v>3</v>
       </c>
@@ -2709,7 +2779,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="120" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:7" ht="44" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B120" s="3">
         <v>4</v>
       </c>
@@ -2727,7 +2797,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="121" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B121" s="11" t="s">
         <v>8</v>
       </c>
@@ -2739,12 +2809,12 @@
       <c r="F121" s="13"/>
       <c r="G121" s="10"/>
     </row>
-    <row r="122" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B123" s="17" t="s">
+    <row r="122" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="123" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B123" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C123" s="18"/>
+      <c r="C123" s="15"/>
       <c r="D123" s="9">
         <v>10</v>
       </c>
@@ -2752,11 +2822,11 @@
       <c r="F123" s="13"/>
       <c r="G123" s="10"/>
     </row>
-    <row r="124" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B124" s="17" t="s">
+    <row r="124" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B124" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C124" s="18"/>
+      <c r="C124" s="15"/>
       <c r="D124" s="9" t="s">
         <v>114</v>
       </c>
@@ -2764,39 +2834,39 @@
       <c r="F124" s="13"/>
       <c r="G124" s="10"/>
     </row>
-    <row r="125" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B125" s="19" t="s">
+    <row r="125" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B125" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C125" s="20"/>
-      <c r="D125" s="23" t="s">
+      <c r="C125" s="17"/>
+      <c r="D125" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E125" s="24"/>
-      <c r="F125" s="24"/>
-      <c r="G125" s="25"/>
-    </row>
-    <row r="126" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B126" s="21"/>
-      <c r="C126" s="22"/>
-      <c r="D126" s="26" t="s">
+      <c r="E125" s="21"/>
+      <c r="F125" s="21"/>
+      <c r="G125" s="22"/>
+    </row>
+    <row r="126" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B126" s="18"/>
+      <c r="C126" s="19"/>
+      <c r="D126" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E126" s="27"/>
-      <c r="F126" s="27"/>
-      <c r="G126" s="28"/>
-    </row>
-    <row r="127" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B127" s="14" t="s">
+      <c r="E126" s="24"/>
+      <c r="F126" s="24"/>
+      <c r="G126" s="25"/>
+    </row>
+    <row r="127" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B127" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
-      <c r="E127" s="15"/>
-      <c r="F127" s="15"/>
-      <c r="G127" s="16"/>
-    </row>
-    <row r="128" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C127" s="27"/>
+      <c r="D127" s="27"/>
+      <c r="E127" s="27"/>
+      <c r="F127" s="27"/>
+      <c r="G127" s="28"/>
+    </row>
+    <row r="128" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B128" s="1" t="s">
         <v>3</v>
       </c>
@@ -2814,7 +2884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B129" s="3">
         <v>1</v>
       </c>
@@ -2832,7 +2902,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="130" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B130" s="3">
         <v>2</v>
       </c>
@@ -2850,7 +2920,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="131" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B131" s="3">
         <v>3</v>
       </c>
@@ -2868,7 +2938,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="132" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B132" s="3">
         <v>4</v>
       </c>
@@ -2886,7 +2956,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="133" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B133" s="3">
         <v>5</v>
       </c>
@@ -2904,7 +2974,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="134" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B134" s="3">
         <v>6</v>
       </c>
@@ -2922,7 +2992,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="135" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B135" s="3">
         <v>7</v>
       </c>
@@ -2940,7 +3010,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B136" s="3">
         <v>8</v>
       </c>
@@ -2958,7 +3028,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="38.700000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:7" ht="38.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B137" s="3">
         <v>9</v>
       </c>
@@ -2976,7 +3046,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="138" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B138" s="11" t="s">
         <v>8</v>
       </c>
@@ -2988,12 +3058,12 @@
       <c r="F138" s="13"/>
       <c r="G138" s="10"/>
     </row>
-    <row r="139" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="140" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B140" s="17" t="s">
+    <row r="139" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="140" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B140" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C140" s="18"/>
+      <c r="C140" s="15"/>
       <c r="D140" s="9">
         <v>11</v>
       </c>
@@ -3001,11 +3071,11 @@
       <c r="F140" s="13"/>
       <c r="G140" s="10"/>
     </row>
-    <row r="141" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B141" s="17" t="s">
+    <row r="141" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B141" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C141" s="18"/>
+      <c r="C141" s="15"/>
       <c r="D141" s="9" t="s">
         <v>144</v>
       </c>
@@ -3013,39 +3083,39 @@
       <c r="F141" s="13"/>
       <c r="G141" s="10"/>
     </row>
-    <row r="142" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B142" s="19" t="s">
+    <row r="142" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B142" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C142" s="20"/>
-      <c r="D142" s="23" t="s">
+      <c r="C142" s="17"/>
+      <c r="D142" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E142" s="24"/>
-      <c r="F142" s="24"/>
-      <c r="G142" s="25"/>
-    </row>
-    <row r="143" spans="2:7" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B143" s="21"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="26" t="s">
+      <c r="E142" s="21"/>
+      <c r="F142" s="21"/>
+      <c r="G142" s="22"/>
+    </row>
+    <row r="143" spans="2:7" ht="14.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B143" s="18"/>
+      <c r="C143" s="19"/>
+      <c r="D143" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E143" s="27"/>
-      <c r="F143" s="27"/>
-      <c r="G143" s="28"/>
-    </row>
-    <row r="144" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B144" s="14" t="s">
+      <c r="E143" s="24"/>
+      <c r="F143" s="24"/>
+      <c r="G143" s="25"/>
+    </row>
+    <row r="144" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B144" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C144" s="15"/>
-      <c r="D144" s="15"/>
-      <c r="E144" s="15"/>
-      <c r="F144" s="15"/>
-      <c r="G144" s="16"/>
-    </row>
-    <row r="145" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C144" s="27"/>
+      <c r="D144" s="27"/>
+      <c r="E144" s="27"/>
+      <c r="F144" s="27"/>
+      <c r="G144" s="28"/>
+    </row>
+    <row r="145" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B145" s="1" t="s">
         <v>3</v>
       </c>
@@ -3063,7 +3133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B146" s="3">
         <v>1</v>
       </c>
@@ -3081,7 +3151,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="147" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B147" s="3">
         <v>2</v>
       </c>
@@ -3099,7 +3169,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="148" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B148" s="3">
         <v>3</v>
       </c>
@@ -3117,7 +3187,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="149" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B149" s="3">
         <v>4</v>
       </c>
@@ -3135,7 +3205,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="150" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B150" s="3">
         <v>5</v>
       </c>
@@ -3153,7 +3223,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="151" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B151" s="3">
         <v>6</v>
       </c>
@@ -3171,7 +3241,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="152" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B152" s="11" t="s">
         <v>8</v>
       </c>
@@ -3183,12 +3253,12 @@
       <c r="F152" s="13"/>
       <c r="G152" s="10"/>
     </row>
-    <row r="153" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="154" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B154" s="17" t="s">
+    <row r="153" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="154" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B154" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C154" s="18"/>
+      <c r="C154" s="15"/>
       <c r="D154" s="9">
         <v>12</v>
       </c>
@@ -3196,11 +3266,11 @@
       <c r="F154" s="13"/>
       <c r="G154" s="10"/>
     </row>
-    <row r="155" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B155" s="17" t="s">
+    <row r="155" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B155" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C155" s="18"/>
+      <c r="C155" s="15"/>
       <c r="D155" s="9" t="s">
         <v>134</v>
       </c>
@@ -3208,39 +3278,39 @@
       <c r="F155" s="13"/>
       <c r="G155" s="10"/>
     </row>
-    <row r="156" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B156" s="19" t="s">
+    <row r="156" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B156" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C156" s="20"/>
-      <c r="D156" s="23" t="s">
+      <c r="C156" s="17"/>
+      <c r="D156" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E156" s="24"/>
-      <c r="F156" s="24"/>
-      <c r="G156" s="25"/>
-    </row>
-    <row r="157" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B157" s="21"/>
-      <c r="C157" s="22"/>
-      <c r="D157" s="26" t="s">
+      <c r="E156" s="21"/>
+      <c r="F156" s="21"/>
+      <c r="G156" s="22"/>
+    </row>
+    <row r="157" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B157" s="18"/>
+      <c r="C157" s="19"/>
+      <c r="D157" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E157" s="27"/>
-      <c r="F157" s="27"/>
-      <c r="G157" s="28"/>
-    </row>
-    <row r="158" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B158" s="14" t="s">
+      <c r="E157" s="24"/>
+      <c r="F157" s="24"/>
+      <c r="G157" s="25"/>
+    </row>
+    <row r="158" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B158" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C158" s="15"/>
-      <c r="D158" s="15"/>
-      <c r="E158" s="15"/>
-      <c r="F158" s="15"/>
-      <c r="G158" s="16"/>
-    </row>
-    <row r="159" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C158" s="27"/>
+      <c r="D158" s="27"/>
+      <c r="E158" s="27"/>
+      <c r="F158" s="27"/>
+      <c r="G158" s="28"/>
+    </row>
+    <row r="159" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B159" s="1" t="s">
         <v>3</v>
       </c>
@@ -3258,7 +3328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B160" s="3">
         <v>1</v>
       </c>
@@ -3276,7 +3346,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="161" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B161" s="3">
         <v>2</v>
       </c>
@@ -3294,7 +3364,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="162" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B162" s="3">
         <v>3</v>
       </c>
@@ -3312,7 +3382,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="163" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B163" s="3">
         <v>4</v>
       </c>
@@ -3330,7 +3400,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="164" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B164" s="3">
         <v>5</v>
       </c>
@@ -3348,7 +3418,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="165" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B165" s="11" t="s">
         <v>8</v>
       </c>
@@ -3360,9 +3430,186 @@
       <c r="F165" s="13"/>
       <c r="G165" s="10"/>
     </row>
-    <row r="166" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="201">
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="D109:G109"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:G100"/>
+    <mergeCell ref="B101:C102"/>
+    <mergeCell ref="D101:G101"/>
+    <mergeCell ref="D102:G102"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="B91:G91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="B89:C90"/>
+    <mergeCell ref="D89:G89"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="D87:G87"/>
+    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="B75:C76"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="D111:G111"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="D112:G112"/>
+    <mergeCell ref="B113:C114"/>
+    <mergeCell ref="D113:G113"/>
+    <mergeCell ref="D114:G114"/>
+    <mergeCell ref="B115:G115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="D123:G123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="D124:G124"/>
+    <mergeCell ref="B125:C126"/>
+    <mergeCell ref="D125:G125"/>
+    <mergeCell ref="D126:G126"/>
+    <mergeCell ref="B144:G144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="C146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="B138:C138"/>
+    <mergeCell ref="D138:G138"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="D140:G140"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="B141:C141"/>
+    <mergeCell ref="D141:G141"/>
+    <mergeCell ref="B142:C143"/>
+    <mergeCell ref="D142:G142"/>
+    <mergeCell ref="D143:G143"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C160:D160"/>
@@ -3387,183 +3634,436 @@
     <mergeCell ref="C149:D149"/>
     <mergeCell ref="B152:C152"/>
     <mergeCell ref="D152:G152"/>
-    <mergeCell ref="B144:G144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="C146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="B138:C138"/>
-    <mergeCell ref="D138:G138"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="D140:G140"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="B141:C141"/>
-    <mergeCell ref="D141:G141"/>
-    <mergeCell ref="B142:C143"/>
-    <mergeCell ref="D142:G142"/>
-    <mergeCell ref="D143:G143"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="D123:G123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="D124:G124"/>
-    <mergeCell ref="B125:C126"/>
-    <mergeCell ref="D125:G125"/>
-    <mergeCell ref="D126:G126"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="D112:G112"/>
-    <mergeCell ref="B113:C114"/>
-    <mergeCell ref="D113:G113"/>
-    <mergeCell ref="D114:G114"/>
-    <mergeCell ref="B115:G115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="D111:G111"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E192BF06-66C7-4B4F-95C1-D1A93166083F}">
+  <dimension ref="B4:G31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.53125" customWidth="1"/>
+    <col min="4" max="4" width="23.9296875" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="9">
+        <v>8</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
+    </row>
+    <row r="8" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="3">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="19" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="9">
+        <v>9</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="45.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="29.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:C34"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:G71"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B77:G77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="B75:C76"/>
-    <mergeCell ref="D75:G75"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B89:C90"/>
-    <mergeCell ref="D89:G89"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:G85"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="D87:G87"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="D109:G109"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:G100"/>
-    <mergeCell ref="B101:C102"/>
-    <mergeCell ref="D101:G101"/>
-    <mergeCell ref="D102:G102"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:G97"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:G99"/>
-    <mergeCell ref="B91:G91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified test cases && word with manual testing
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csd\Desktop\products\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3AAD2A-67B0-4E33-8021-9B6D8291BCC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D4128DB-3984-4398-B733-45B1C1BFEEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="199">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Se afișează pagina de înregistrare a contului</t>
   </si>
   <si>
-    <t>Utilizatorul este redirecționat către pagina coșului de cumpărături</t>
-  </si>
-  <si>
     <t>Utilizatorul va avea un cont nou pe platforma Zooplus</t>
   </si>
   <si>
@@ -620,6 +617,12 @@
   </si>
   <si>
     <t>Se verifica de catre utilizator dacă reducerea de 5% a fost aplicată automat</t>
+  </si>
+  <si>
+    <t>Se selecteaza voucherul pentru produsul dorit</t>
+  </si>
+  <si>
+    <t>Voucherul aferent produsului este selectat</t>
   </si>
 </sst>
 </file>
@@ -941,19 +944,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -965,6 +962,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -985,6 +988,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -992,21 +1010,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1292,8 +1295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86:C86"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,10 +1311,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="9">
         <v>1</v>
       </c>
@@ -1320,10 +1323,10 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="15"/>
+      <c r="C3" s="12"/>
       <c r="D3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1332,10 +1335,10 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="20" t="s">
         <v>10</v>
       </c>
@@ -1344,8 +1347,8 @@
       <c r="G4" s="22"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
       <c r="D5" s="23" t="s">
         <v>11</v>
       </c>
@@ -1354,23 +1357,23 @@
       <c r="G5" s="25"/>
     </row>
     <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1386,7 +1389,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="4" t="s">
@@ -1400,11 +1403,11 @@
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
@@ -1414,7 +1417,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="4" t="s">
@@ -1456,7 +1459,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
@@ -1466,10 +1469,10 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="12"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1479,10 +1482,10 @@
     </row>
     <row r="15" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="9">
         <v>2</v>
       </c>
@@ -1491,22 +1494,22 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="20" t="s">
         <v>10</v>
       </c>
@@ -1515,8 +1518,8 @@
       <c r="G18" s="22"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="23" t="s">
         <v>20</v>
       </c>
@@ -1525,33 +1528,33 @@
       <c r="G19" s="25"/>
     </row>
     <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
     </row>
     <row r="21" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1567,7 +1570,7 @@
         <v>1</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="4" t="s">
@@ -1581,7 +1584,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="4" t="s">
@@ -1595,7 +1598,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="4" t="s">
@@ -1637,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
@@ -1647,10 +1650,10 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="30"/>
       <c r="D29" s="9" t="s">
         <v>29</v>
       </c>
@@ -1660,10 +1663,10 @@
     </row>
     <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="9">
         <v>3</v>
       </c>
@@ -1672,22 +1675,22 @@
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="17"/>
+      <c r="C33" s="15"/>
       <c r="D33" s="20" t="s">
         <v>10</v>
       </c>
@@ -1696,8 +1699,8 @@
       <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="23" t="s">
         <v>20</v>
       </c>
@@ -1706,23 +1709,23 @@
       <c r="G34" s="25"/>
     </row>
     <row r="35" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="33"/>
     </row>
     <row r="36" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1738,7 +1741,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="4" t="s">
@@ -1748,7 +1751,7 @@
         <v>12</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1766,7 +1769,7 @@
         <v>32</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1784,7 +1787,7 @@
         <v>34</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1792,7 +1795,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="4" t="s">
@@ -1802,7 +1805,7 @@
         <v>35</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1810,17 +1813,17 @@
         <v>5</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1828,17 +1831,17 @@
         <v>6</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1853,17 +1856,17 @@
         <v>38</v>
       </c>
       <c r="F43" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="8" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="44" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="12"/>
+      <c r="C44" s="30"/>
       <c r="D44" s="9" t="s">
         <v>39</v>
       </c>
@@ -1873,10 +1876,10 @@
     </row>
     <row r="45" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="15"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="9">
         <v>4</v>
       </c>
@@ -1885,22 +1888,22 @@
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="12"/>
       <c r="D47" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="15"/>
       <c r="D48" s="20" t="s">
         <v>10</v>
       </c>
@@ -1909,8 +1912,8 @@
       <c r="G48" s="22"/>
     </row>
     <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="17"/>
       <c r="D49" s="23" t="s">
         <v>20</v>
       </c>
@@ -1919,23 +1922,23 @@
       <c r="G49" s="25"/>
     </row>
     <row r="50" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="28"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="33"/>
     </row>
     <row r="51" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="12"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="2" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="4" t="s">
@@ -1961,7 +1964,7 @@
         <v>12</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1969,7 +1972,7 @@
         <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="4" t="s">
@@ -1979,7 +1982,7 @@
         <v>40</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1987,7 +1990,7 @@
         <v>3</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="4" t="s">
@@ -1997,7 +2000,7 @@
         <v>41</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2015,7 +2018,7 @@
         <v>43</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2023,7 +2026,7 @@
         <v>5</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="4" t="s">
@@ -2033,7 +2036,7 @@
         <v>44</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2051,14 +2054,14 @@
         <v>46</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="12"/>
+      <c r="C58" s="30"/>
       <c r="D58" s="9" t="s">
         <v>47</v>
       </c>
@@ -2068,10 +2071,10 @@
     </row>
     <row r="59" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="15"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="9">
         <v>5</v>
       </c>
@@ -2080,10 +2083,10 @@
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="15"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="9" t="s">
         <v>48</v>
       </c>
@@ -2092,10 +2095,10 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="17"/>
+      <c r="C62" s="15"/>
       <c r="D62" s="20" t="s">
         <v>10</v>
       </c>
@@ -2104,8 +2107,8 @@
       <c r="G62" s="22"/>
     </row>
     <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="18"/>
-      <c r="C63" s="19"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="17"/>
       <c r="D63" s="23" t="s">
         <v>49</v>
       </c>
@@ -2114,23 +2117,23 @@
       <c r="G63" s="25"/>
     </row>
     <row r="64" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="28"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="32"/>
+      <c r="G64" s="33"/>
     </row>
     <row r="65" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="12"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2169,155 +2172,155 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="3">
         <v>3</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="3">
         <v>4</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="4" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="3">
-        <v>5</v>
-      </c>
-      <c r="C70" s="9" t="s">
+    <row r="70" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" s="30"/>
+      <c r="D70" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="9">
+        <v>6</v>
+      </c>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="D70" s="10"/>
-      <c r="E70" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="F70" s="4"/>
-      <c r="G70" s="5"/>
-    </row>
-    <row r="71" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="10"/>
-    </row>
-    <row r="72" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" s="15"/>
-      <c r="D73" s="9">
-        <v>6</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C74" s="15"/>
-      <c r="D74" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="10"/>
-    </row>
-    <row r="75" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="16" t="s">
+      <c r="D74" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="22"/>
+    </row>
+    <row r="75" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="16"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="25"/>
+    </row>
+    <row r="76" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="32"/>
+      <c r="G76" s="33"/>
+    </row>
+    <row r="77" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C77" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="30"/>
+      <c r="E77" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="3">
         <v>1</v>
       </c>
-      <c r="C75" s="17"/>
-      <c r="D75" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="22"/>
-    </row>
-    <row r="76" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="18"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="25"/>
-    </row>
-    <row r="77" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="26" t="s">
+      <c r="C78" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F78" s="4"/>
+      <c r="G78" s="5"/>
+    </row>
+    <row r="79" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="3">
         <v>2</v>
       </c>
-      <c r="C77" s="27"/>
-      <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
-      <c r="F77" s="27"/>
-      <c r="G77" s="28"/>
-    </row>
-    <row r="78" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="3">
-        <v>1</v>
-      </c>
       <c r="C79" s="9" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D79" s="10"/>
       <c r="E79" s="4" t="s">
-        <v>51</v>
+        <v>172</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
     <row r="80" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="D80" s="10"/>
       <c r="E80" s="4" t="s">
@@ -2326,37 +2329,37 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D81" s="10"/>
       <c r="E81" s="4" t="s">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
     <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>64</v>
+        <v>197</v>
       </c>
       <c r="D82" s="10"/>
       <c r="E82" s="4" t="s">
-        <v>65</v>
+        <v>198</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
     <row r="83" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>16</v>
@@ -2370,39 +2373,39 @@
     </row>
     <row r="84" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="2:7" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B85" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="12"/>
+      <c r="C86" s="30"/>
       <c r="D86" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
@@ -2410,10 +2413,10 @@
     </row>
     <row r="87" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="15"/>
+      <c r="C88" s="12"/>
       <c r="D88" s="9">
         <v>7</v>
       </c>
@@ -2422,22 +2425,22 @@
       <c r="G88" s="10"/>
     </row>
     <row r="89" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="15"/>
+      <c r="C89" s="12"/>
       <c r="D89" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="10"/>
     </row>
     <row r="90" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C90" s="17"/>
+      <c r="C90" s="15"/>
       <c r="D90" s="20" t="s">
         <v>10</v>
       </c>
@@ -2446,33 +2449,33 @@
       <c r="G90" s="22"/>
     </row>
     <row r="91" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="18"/>
-      <c r="C91" s="19"/>
+      <c r="B91" s="16"/>
+      <c r="C91" s="17"/>
       <c r="D91" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E91" s="24"/>
       <c r="F91" s="24"/>
       <c r="G91" s="25"/>
     </row>
     <row r="92" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="26" t="s">
+      <c r="B92" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="27"/>
-      <c r="D92" s="27"/>
-      <c r="E92" s="27"/>
-      <c r="F92" s="27"/>
-      <c r="G92" s="28"/>
+      <c r="C92" s="32"/>
+      <c r="D92" s="32"/>
+      <c r="E92" s="32"/>
+      <c r="F92" s="32"/>
+      <c r="G92" s="33"/>
     </row>
     <row r="93" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="11" t="s">
+      <c r="C93" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="12"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2502,11 +2505,11 @@
         <v>2</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
@@ -2516,11 +2519,11 @@
         <v>3</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D96" s="10"/>
       <c r="E96" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
@@ -2530,11 +2533,11 @@
         <v>4</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D97" s="10"/>
       <c r="E97" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
@@ -2544,11 +2547,11 @@
         <v>5</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D98" s="10"/>
       <c r="E98" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
@@ -2558,11 +2561,11 @@
         <v>6</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D99" s="10"/>
       <c r="E99" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
@@ -2572,22 +2575,22 @@
         <v>7</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D100" s="10"/>
       <c r="E100" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
     <row r="101" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="11" t="s">
+      <c r="B101" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="12"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
@@ -2595,10 +2598,10 @@
     </row>
     <row r="102" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="15"/>
+      <c r="C103" s="12"/>
       <c r="D103" s="9">
         <v>8</v>
       </c>
@@ -2607,22 +2610,22 @@
       <c r="G103" s="10"/>
     </row>
     <row r="104" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="15"/>
+      <c r="C104" s="12"/>
       <c r="D104" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="10"/>
     </row>
     <row r="105" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="16" t="s">
+      <c r="B105" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="17"/>
+      <c r="C105" s="15"/>
       <c r="D105" s="20" t="s">
         <v>10</v>
       </c>
@@ -2631,33 +2634,33 @@
       <c r="G105" s="22"/>
     </row>
     <row r="106" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="18"/>
-      <c r="C106" s="19"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="17"/>
       <c r="D106" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E106" s="24"/>
       <c r="F106" s="24"/>
       <c r="G106" s="25"/>
     </row>
     <row r="107" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="26" t="s">
+      <c r="B107" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="27"/>
-      <c r="D107" s="27"/>
-      <c r="E107" s="27"/>
-      <c r="F107" s="27"/>
-      <c r="G107" s="28"/>
+      <c r="C107" s="32"/>
+      <c r="D107" s="32"/>
+      <c r="E107" s="32"/>
+      <c r="F107" s="32"/>
+      <c r="G107" s="33"/>
     </row>
     <row r="108" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="11" t="s">
+      <c r="C108" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="12"/>
+      <c r="D108" s="30"/>
       <c r="E108" s="2" t="s">
         <v>5</v>
       </c>
@@ -2687,11 +2690,11 @@
         <v>2</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
@@ -2701,11 +2704,11 @@
         <v>3</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D111" s="10"/>
       <c r="E111" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
@@ -2715,11 +2718,11 @@
         <v>4</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D112" s="10"/>
       <c r="E112" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
@@ -2729,11 +2732,11 @@
         <v>5</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D113" s="10"/>
       <c r="E113" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
@@ -2743,11 +2746,11 @@
         <v>6</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D114" s="10"/>
       <c r="E114" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
@@ -2757,22 +2760,22 @@
         <v>7</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D115" s="10"/>
       <c r="E115" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F115" s="4"/>
       <c r="G115" s="5"/>
     </row>
     <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C116" s="12"/>
+      <c r="C116" s="30"/>
       <c r="D116" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
@@ -2780,10 +2783,10 @@
     </row>
     <row r="117" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="14" t="s">
+      <c r="B118" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C118" s="15"/>
+      <c r="C118" s="12"/>
       <c r="D118" s="9">
         <v>9</v>
       </c>
@@ -2792,22 +2795,22 @@
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C119" s="15"/>
+      <c r="C119" s="12"/>
       <c r="D119" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="10"/>
     </row>
     <row r="120" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="16" t="s">
+      <c r="B120" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="17"/>
+      <c r="C120" s="15"/>
       <c r="D120" s="20" t="s">
         <v>10</v>
       </c>
@@ -2816,33 +2819,33 @@
       <c r="G120" s="22"/>
     </row>
     <row r="121" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="18"/>
-      <c r="C121" s="19"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="17"/>
       <c r="D121" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E121" s="24"/>
       <c r="F121" s="24"/>
       <c r="G121" s="25"/>
     </row>
     <row r="122" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="26" t="s">
+      <c r="B122" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="27"/>
-      <c r="G122" s="28"/>
+      <c r="C122" s="32"/>
+      <c r="D122" s="32"/>
+      <c r="E122" s="32"/>
+      <c r="F122" s="32"/>
+      <c r="G122" s="33"/>
     </row>
     <row r="123" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="11" t="s">
+      <c r="C123" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="12"/>
+      <c r="D123" s="30"/>
       <c r="E123" s="2" t="s">
         <v>5</v>
       </c>
@@ -2858,17 +2861,17 @@
         <v>1</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2876,17 +2879,17 @@
         <v>2</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D125" s="10"/>
       <c r="E125" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2894,17 +2897,17 @@
         <v>3</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2912,26 +2915,26 @@
         <v>4</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="11" t="s">
+      <c r="B128" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="12"/>
+      <c r="C128" s="30"/>
       <c r="D128" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
@@ -2939,10 +2942,10 @@
     </row>
     <row r="129" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="15"/>
+      <c r="C130" s="12"/>
       <c r="D130" s="9">
         <v>10</v>
       </c>
@@ -2951,22 +2954,22 @@
       <c r="G130" s="10"/>
     </row>
     <row r="131" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C131" s="15"/>
+      <c r="C131" s="12"/>
       <c r="D131" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E131" s="13"/>
       <c r="F131" s="13"/>
       <c r="G131" s="10"/>
     </row>
     <row r="132" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="16" t="s">
+      <c r="B132" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C132" s="17"/>
+      <c r="C132" s="15"/>
       <c r="D132" s="20" t="s">
         <v>10</v>
       </c>
@@ -2975,33 +2978,33 @@
       <c r="G132" s="22"/>
     </row>
     <row r="133" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="18"/>
-      <c r="C133" s="19"/>
+      <c r="B133" s="16"/>
+      <c r="C133" s="17"/>
       <c r="D133" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E133" s="24"/>
       <c r="F133" s="24"/>
       <c r="G133" s="25"/>
     </row>
     <row r="134" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="26" t="s">
+      <c r="B134" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="27"/>
-      <c r="D134" s="27"/>
-      <c r="E134" s="27"/>
-      <c r="F134" s="27"/>
-      <c r="G134" s="28"/>
+      <c r="C134" s="32"/>
+      <c r="D134" s="32"/>
+      <c r="E134" s="32"/>
+      <c r="F134" s="32"/>
+      <c r="G134" s="33"/>
     </row>
     <row r="135" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="11" t="s">
+      <c r="C135" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="12"/>
+      <c r="D135" s="30"/>
       <c r="E135" s="2" t="s">
         <v>5</v>
       </c>
@@ -3017,17 +3020,17 @@
         <v>1</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D136" s="10"/>
       <c r="E136" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3035,17 +3038,17 @@
         <v>2</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D137" s="10"/>
       <c r="E137" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3053,17 +3056,17 @@
         <v>3</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D138" s="10"/>
       <c r="E138" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3071,17 +3074,17 @@
         <v>4</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D139" s="10"/>
       <c r="E139" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="140" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3089,17 +3092,17 @@
         <v>5</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D140" s="10"/>
       <c r="E140" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3107,17 +3110,17 @@
         <v>6</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D141" s="10"/>
       <c r="E141" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="142" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3125,17 +3128,17 @@
         <v>7</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D142" s="10"/>
       <c r="E142" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="143" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,17 +3146,17 @@
         <v>8</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D143" s="10"/>
       <c r="E143" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="144" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3161,26 +3164,26 @@
         <v>9</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D144" s="10"/>
       <c r="E144" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="145" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="11" t="s">
+      <c r="B145" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="12"/>
+      <c r="C145" s="30"/>
       <c r="D145" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E145" s="13"/>
       <c r="F145" s="13"/>
@@ -3188,10 +3191,10 @@
     </row>
     <row r="146" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="147" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="14" t="s">
+      <c r="B147" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C147" s="15"/>
+      <c r="C147" s="12"/>
       <c r="D147" s="9">
         <v>11</v>
       </c>
@@ -3200,22 +3203,22 @@
       <c r="G147" s="10"/>
     </row>
     <row r="148" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="14" t="s">
+      <c r="B148" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="15"/>
+      <c r="C148" s="12"/>
       <c r="D148" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E148" s="13"/>
       <c r="F148" s="13"/>
       <c r="G148" s="10"/>
     </row>
     <row r="149" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="16" t="s">
+      <c r="B149" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C149" s="17"/>
+      <c r="C149" s="15"/>
       <c r="D149" s="20" t="s">
         <v>10</v>
       </c>
@@ -3224,33 +3227,33 @@
       <c r="G149" s="22"/>
     </row>
     <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="18"/>
-      <c r="C150" s="19"/>
+      <c r="B150" s="16"/>
+      <c r="C150" s="17"/>
       <c r="D150" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E150" s="24"/>
       <c r="F150" s="24"/>
       <c r="G150" s="25"/>
     </row>
     <row r="151" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="26" t="s">
+      <c r="B151" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C151" s="27"/>
-      <c r="D151" s="27"/>
-      <c r="E151" s="27"/>
-      <c r="F151" s="27"/>
-      <c r="G151" s="28"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="32"/>
+      <c r="E151" s="32"/>
+      <c r="F151" s="32"/>
+      <c r="G151" s="33"/>
     </row>
     <row r="152" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B152" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C152" s="11" t="s">
+      <c r="C152" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D152" s="12"/>
+      <c r="D152" s="30"/>
       <c r="E152" s="2" t="s">
         <v>5</v>
       </c>
@@ -3266,17 +3269,17 @@
         <v>1</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D153" s="10"/>
       <c r="E153" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="154" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3284,17 +3287,17 @@
         <v>2</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D154" s="10"/>
       <c r="E154" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="155" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3302,17 +3305,17 @@
         <v>3</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D155" s="10"/>
       <c r="E155" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G155" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="156" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3320,17 +3323,17 @@
         <v>4</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D156" s="10"/>
       <c r="E156" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G156" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="157" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3338,17 +3341,17 @@
         <v>5</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D157" s="10"/>
       <c r="E157" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G157" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="158" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3356,26 +3359,26 @@
         <v>6</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D158" s="10"/>
       <c r="E158" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G158" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159" s="30"/>
+      <c r="D159" s="9" t="s">
         <v>135</v>
-      </c>
-      <c r="F158" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G158" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C159" s="12"/>
-      <c r="D159" s="9" t="s">
-        <v>136</v>
       </c>
       <c r="E159" s="13"/>
       <c r="F159" s="13"/>
@@ -3383,10 +3386,10 @@
     </row>
     <row r="160" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="161" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="14" t="s">
+      <c r="B161" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="15"/>
+      <c r="C161" s="12"/>
       <c r="D161" s="9">
         <v>12</v>
       </c>
@@ -3395,22 +3398,22 @@
       <c r="G161" s="10"/>
     </row>
     <row r="162" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="14" t="s">
+      <c r="B162" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="15"/>
+      <c r="C162" s="12"/>
       <c r="D162" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E162" s="13"/>
       <c r="F162" s="13"/>
       <c r="G162" s="10"/>
     </row>
     <row r="163" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="16" t="s">
+      <c r="B163" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C163" s="17"/>
+      <c r="C163" s="15"/>
       <c r="D163" s="20" t="s">
         <v>10</v>
       </c>
@@ -3419,33 +3422,33 @@
       <c r="G163" s="22"/>
     </row>
     <row r="164" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="18"/>
-      <c r="C164" s="19"/>
+      <c r="B164" s="16"/>
+      <c r="C164" s="17"/>
       <c r="D164" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E164" s="24"/>
       <c r="F164" s="24"/>
       <c r="G164" s="25"/>
     </row>
     <row r="165" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="26" t="s">
+      <c r="B165" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="27"/>
-      <c r="D165" s="27"/>
-      <c r="E165" s="27"/>
-      <c r="F165" s="27"/>
-      <c r="G165" s="28"/>
+      <c r="C165" s="32"/>
+      <c r="D165" s="32"/>
+      <c r="E165" s="32"/>
+      <c r="F165" s="32"/>
+      <c r="G165" s="33"/>
     </row>
     <row r="166" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B166" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C166" s="11" t="s">
+      <c r="C166" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="12"/>
+      <c r="D166" s="30"/>
       <c r="E166" s="2" t="s">
         <v>5</v>
       </c>
@@ -3461,17 +3464,17 @@
         <v>1</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D167" s="10"/>
       <c r="E167" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="168" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3479,17 +3482,17 @@
         <v>2</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D168" s="10"/>
       <c r="E168" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="169" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3497,17 +3500,17 @@
         <v>3</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D169" s="10"/>
       <c r="E169" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G169" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="170" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3515,17 +3518,17 @@
         <v>4</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D170" s="10"/>
       <c r="E170" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="171" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3533,26 +3536,26 @@
         <v>5</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D171" s="10"/>
       <c r="E171" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G171" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B172" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172" s="30"/>
+      <c r="D172" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="F171" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G171" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="172" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C172" s="12"/>
-      <c r="D172" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="E172" s="13"/>
       <c r="F172" s="13"/>
@@ -3564,8 +3567,8 @@
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="B116:C116"/>
     <mergeCell ref="D116:G116"/>
+    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C82:D82"/>
     <mergeCell ref="B107:G107"/>
     <mergeCell ref="C108:D108"/>
     <mergeCell ref="C109:D109"/>
@@ -3596,22 +3599,22 @@
     <mergeCell ref="D86:G86"/>
     <mergeCell ref="B88:C88"/>
     <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B77:G77"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="C77:D77"/>
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="B75:C76"/>
-    <mergeCell ref="D75:G75"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:G71"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="D73:G73"/>
+    <mergeCell ref="B74:C75"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:G72"/>
     <mergeCell ref="B64:G64"/>
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
@@ -3778,7 +3781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E192BF06-66C7-4B4F-95C1-D1A93166083F}">
   <dimension ref="B4:G31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -3793,10 +3796,10 @@
   <sheetData>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="15"/>
+      <c r="C5" s="12"/>
       <c r="D5" s="9">
         <v>8</v>
       </c>
@@ -3805,22 +3808,22 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="12"/>
       <c r="D6" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="10"/>
     </row>
     <row r="7" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="20" t="s">
         <v>10</v>
       </c>
@@ -3829,33 +3832,33 @@
       <c r="G7" s="22"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3871,17 +3874,17 @@
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3889,17 +3892,17 @@
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3907,17 +3910,17 @@
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3925,17 +3928,17 @@
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3943,17 +3946,17 @@
         <v>5</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3961,26 +3964,26 @@
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
@@ -3988,10 +3991,10 @@
     </row>
     <row r="18" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="9">
         <v>9</v>
       </c>
@@ -4000,22 +4003,22 @@
       <c r="G19" s="10"/>
     </row>
     <row r="20" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="17"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="20" t="s">
         <v>10</v>
       </c>
@@ -4024,33 +4027,33 @@
       <c r="G21" s="22"/>
     </row>
     <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="25"/>
     </row>
     <row r="23" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="33"/>
     </row>
     <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="2" t="s">
         <v>5</v>
       </c>
@@ -4066,17 +4069,17 @@
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4084,17 +4087,17 @@
         <v>2</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4102,17 +4105,17 @@
         <v>3</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="29.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4120,17 +4123,17 @@
         <v>4</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4138,26 +4141,26 @@
         <v>5</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="9" t="s">
         <v>167</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="9" t="s">
-        <v>168</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>

</xml_diff>

<commit_message>
Added another 2 performance test cases and updated formatting in the word document
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csd\Desktop\products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Computer\Master\An 1\Semestru 2\Testarea aplicatiilor software TAS\Proiect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D4128DB-3984-4398-B733-45B1C1BFEEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C2BB24-30DF-4793-9FE3-4DFE2407A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testarea funcțională" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="218">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -623,6 +623,63 @@
   </si>
   <si>
     <t>Voucherul aferent produsului este selectat</t>
+  </si>
+  <si>
+    <t>Utilizatorul are cel puțin un produs în coș</t>
+  </si>
+  <si>
+    <t>Se apasă pe iconița cu coșul de cumpărături</t>
+  </si>
+  <si>
+    <t>Se afișează o fereastră cu coșul de cumpărături</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul "COȘUL DE CUMPĂRĂTURI"</t>
+  </si>
+  <si>
+    <t>Se redirecționează la pagina coșului de cumpărături</t>
+  </si>
+  <si>
+    <t>Maxi Pet - Creșterea cantității și apoi eliminara unui produs din coșul de cumpărături</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul cu + pentru creșterea cantității unui produs</t>
+  </si>
+  <si>
+    <t>Cantitatea este incrementată cu o unitate</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul "Elimină" din dreptul produsului</t>
+  </si>
+  <si>
+    <t>Produsul este eliminat din coș</t>
+  </si>
+  <si>
+    <t>Coșul de cumpărături nu mai conține produsul eliminat</t>
+  </si>
+  <si>
+    <t>Maxi Pet - Filtrare produs căutat</t>
+  </si>
+  <si>
+    <t>Se extinde bara de căutare</t>
+  </si>
+  <si>
+    <t>Se caută după "hrana umeda pisici"</t>
+  </si>
+  <si>
+    <t>Se listează toate produsele ce au legătură cu hrana umedă pentru pisici</t>
+  </si>
+  <si>
+    <t>Se filtrează după opțiunea "hrană uscată"</t>
+  </si>
+  <si>
+    <t>Lista afișată de golește</t>
+  </si>
+  <si>
+    <t>Se afișează hrană uscată pentru pisici, deși căutarea după hrană umedă încă este activă</t>
+  </si>
+  <si>
+    <t>Lista afișată reflectă atât textul din căutare cât și filtrele selectate</t>
   </si>
 </sst>
 </file>
@@ -944,13 +1001,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -962,12 +1034,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -988,6 +1054,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -995,21 +1067,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1295,26 +1352,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:G47"/>
+    <sheetView topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.1328125" customWidth="1"/>
+    <col min="3" max="3" width="15.86328125" customWidth="1"/>
+    <col min="4" max="4" width="33.86328125" customWidth="1"/>
+    <col min="5" max="5" width="22.1328125" customWidth="1"/>
+    <col min="6" max="6" width="29.86328125" customWidth="1"/>
+    <col min="7" max="7" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="9">
         <v>1</v>
       </c>
@@ -1322,11 +1379,11 @@
       <c r="F2" s="13"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="9" t="s">
         <v>30</v>
       </c>
@@ -1334,46 +1391,46 @@
       <c r="F3" s="13"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="23" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1384,7 +1441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -1398,7 +1455,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="3">
         <v>2</v>
       </c>
@@ -1412,7 +1469,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B10" s="3">
         <v>3</v>
       </c>
@@ -1426,7 +1483,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="3">
         <v>4</v>
       </c>
@@ -1440,7 +1497,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="3">
         <v>5</v>
       </c>
@@ -1454,7 +1511,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B13" s="3">
         <v>6</v>
       </c>
@@ -1468,11 +1525,11 @@
       <c r="F13" s="4"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+    <row r="14" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1480,12 +1537,12 @@
       <c r="F14" s="13"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
+    <row r="15" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="9">
         <v>2</v>
       </c>
@@ -1493,11 +1550,11 @@
       <c r="F16" s="13"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="9" t="s">
         <v>70</v>
       </c>
@@ -1505,56 +1562,56 @@
       <c r="F17" s="13"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-    </row>
-    <row r="21" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-    </row>
-    <row r="22" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1565,7 +1622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="3">
         <v>1</v>
       </c>
@@ -1579,7 +1636,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B24" s="3">
         <v>2</v>
       </c>
@@ -1593,7 +1650,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="3">
         <v>3</v>
       </c>
@@ -1607,7 +1664,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B26" s="3">
         <v>4</v>
       </c>
@@ -1621,7 +1678,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="3">
         <v>5</v>
       </c>
@@ -1635,7 +1692,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B28" s="3">
         <v>6</v>
       </c>
@@ -1649,11 +1706,11 @@
       <c r="F28" s="4"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+    <row r="29" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="9" t="s">
         <v>29</v>
       </c>
@@ -1661,12 +1718,12 @@
       <c r="F29" s="13"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+    <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="31" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="9">
         <v>3</v>
       </c>
@@ -1674,11 +1731,11 @@
       <c r="F31" s="13"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
+    <row r="32" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="9" t="s">
         <v>71</v>
       </c>
@@ -1686,46 +1743,46 @@
       <c r="F32" s="13"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B33" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="20" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-    </row>
-    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="23" t="s">
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
+    </row>
+    <row r="34" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-    </row>
-    <row r="35" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="31" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-    </row>
-    <row r="36" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1736,7 +1793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B37" s="3">
         <v>1</v>
       </c>
@@ -1754,7 +1811,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B38" s="3">
         <v>2</v>
       </c>
@@ -1772,7 +1829,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B39" s="3">
         <v>3</v>
       </c>
@@ -1790,7 +1847,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B40" s="3">
         <v>4</v>
       </c>
@@ -1808,7 +1865,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B41" s="3">
         <v>5</v>
       </c>
@@ -1826,7 +1883,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B42" s="3">
         <v>6</v>
       </c>
@@ -1844,7 +1901,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B43" s="3">
         <v>7</v>
       </c>
@@ -1862,11 +1919,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="29" t="s">
+    <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="9" t="s">
         <v>39</v>
       </c>
@@ -1874,12 +1931,12 @@
       <c r="F44" s="13"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="11" t="s">
+    <row r="45" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B46" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="9">
         <v>4</v>
       </c>
@@ -1887,11 +1944,11 @@
       <c r="F46" s="13"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
+    <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B47" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="9" t="s">
         <v>72</v>
       </c>
@@ -1899,46 +1956,46 @@
       <c r="F47" s="13"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+    <row r="48" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B48" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="20" t="s">
+      <c r="C48" s="20"/>
+      <c r="D48" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="16"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="23" t="s">
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="25"/>
+    </row>
+    <row r="49" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
-    </row>
-    <row r="50" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="31" t="s">
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="28"/>
+    </row>
+    <row r="50" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B50" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
-    </row>
-    <row r="51" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="16"/>
+    </row>
+    <row r="51" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="2" t="s">
         <v>5</v>
       </c>
@@ -1949,7 +2006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B52" s="3">
         <v>1</v>
       </c>
@@ -1967,7 +2024,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B53" s="3">
         <v>2</v>
       </c>
@@ -1985,7 +2042,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B54" s="3">
         <v>3</v>
       </c>
@@ -2003,7 +2060,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B55" s="3">
         <v>4</v>
       </c>
@@ -2021,7 +2078,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B56" s="3">
         <v>5</v>
       </c>
@@ -2039,7 +2096,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B57" s="3">
         <v>6</v>
       </c>
@@ -2057,11 +2114,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29" t="s">
+    <row r="58" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B58" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="30"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="9" t="s">
         <v>47</v>
       </c>
@@ -2069,12 +2126,12 @@
       <c r="F58" s="13"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="11" t="s">
+    <row r="59" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="60" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B60" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="18"/>
       <c r="D60" s="9">
         <v>5</v>
       </c>
@@ -2082,11 +2139,11 @@
       <c r="F60" s="13"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="11" t="s">
+    <row r="61" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B61" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="12"/>
+      <c r="C61" s="18"/>
       <c r="D61" s="9" t="s">
         <v>48</v>
       </c>
@@ -2094,46 +2151,46 @@
       <c r="F61" s="13"/>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
+    <row r="62" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B62" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="20"/>
+      <c r="D62" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="16"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="23" t="s">
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
+    </row>
+    <row r="63" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
-    </row>
-    <row r="64" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="31" t="s">
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="28"/>
+    </row>
+    <row r="64" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B64" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
-    </row>
-    <row r="65" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="16"/>
+    </row>
+    <row r="65" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="30"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2144,7 +2201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B66" s="3">
         <v>1</v>
       </c>
@@ -2158,7 +2215,7 @@
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B67" s="3">
         <v>2</v>
       </c>
@@ -2172,7 +2229,7 @@
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B68" s="3">
         <v>3</v>
       </c>
@@ -2186,7 +2243,7 @@
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B69" s="3">
         <v>4</v>
       </c>
@@ -2200,11 +2257,11 @@
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="29" t="s">
+    <row r="70" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B70" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="30"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="9" t="s">
         <v>54</v>
       </c>
@@ -2212,12 +2269,12 @@
       <c r="F70" s="13"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="11" t="s">
+    <row r="71" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="72" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B72" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="12"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="9">
         <v>6</v>
       </c>
@@ -2225,11 +2282,11 @@
       <c r="F72" s="13"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="11" t="s">
+    <row r="73" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B73" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="12"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="9" t="s">
         <v>61</v>
       </c>
@@ -2237,46 +2294,46 @@
       <c r="F73" s="13"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
+    <row r="74" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B74" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="20"/>
+      <c r="D74" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="22"/>
-    </row>
-    <row r="75" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="16"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="23" t="s">
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="25"/>
+    </row>
+    <row r="75" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
-    </row>
-    <row r="76" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="31" t="s">
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="28"/>
+    </row>
+    <row r="76" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B76" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33"/>
-    </row>
-    <row r="77" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="16"/>
+    </row>
+    <row r="77" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="30"/>
+      <c r="D77" s="12"/>
       <c r="E77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2287,7 +2344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B78" s="3">
         <v>1</v>
       </c>
@@ -2301,7 +2358,7 @@
       <c r="F78" s="4"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B79" s="3">
         <v>2</v>
       </c>
@@ -2315,7 +2372,7 @@
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B80" s="3">
         <v>3</v>
       </c>
@@ -2329,7 +2386,7 @@
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B81" s="3">
         <v>4</v>
       </c>
@@ -2343,7 +2400,7 @@
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B82" s="3">
         <v>5</v>
       </c>
@@ -2357,7 +2414,7 @@
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B83" s="3">
         <v>6</v>
       </c>
@@ -2371,7 +2428,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B84" s="3">
         <v>7</v>
       </c>
@@ -2385,7 +2442,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="2:7" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B85" s="3">
         <v>8</v>
       </c>
@@ -2399,11 +2456,11 @@
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="29" t="s">
+    <row r="86" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B86" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="30"/>
+      <c r="C86" s="12"/>
       <c r="D86" s="9" t="s">
         <v>91</v>
       </c>
@@ -2411,12 +2468,12 @@
       <c r="F86" s="13"/>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="11" t="s">
+    <row r="87" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="88" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B88" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="12"/>
+      <c r="C88" s="18"/>
       <c r="D88" s="9">
         <v>7</v>
       </c>
@@ -2424,11 +2481,11 @@
       <c r="F88" s="13"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="11" t="s">
+    <row r="89" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="12"/>
+      <c r="C89" s="18"/>
       <c r="D89" s="9" t="s">
         <v>56</v>
       </c>
@@ -2436,46 +2493,46 @@
       <c r="F89" s="13"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="14" t="s">
+    <row r="90" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B90" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20" t="s">
+      <c r="C90" s="20"/>
+      <c r="D90" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="22"/>
-    </row>
-    <row r="91" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="16"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="23" t="s">
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
+    </row>
+    <row r="91" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
-    </row>
-    <row r="92" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="31" t="s">
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="28"/>
+    </row>
+    <row r="92" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B92" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
-    </row>
-    <row r="93" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="16"/>
+    </row>
+    <row r="93" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="29" t="s">
+      <c r="C93" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="30"/>
+      <c r="D93" s="12"/>
       <c r="E93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2486,7 +2543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B94" s="3">
         <v>1</v>
       </c>
@@ -2500,7 +2557,7 @@
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B95" s="3">
         <v>2</v>
       </c>
@@ -2514,7 +2571,7 @@
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="2:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B96" s="3">
         <v>3</v>
       </c>
@@ -2528,7 +2585,7 @@
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="2:7" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B97" s="3">
         <v>4</v>
       </c>
@@ -2542,7 +2599,7 @@
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B98" s="3">
         <v>5</v>
       </c>
@@ -2556,7 +2613,7 @@
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B99" s="3">
         <v>6</v>
       </c>
@@ -2570,7 +2627,7 @@
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B100" s="3">
         <v>7</v>
       </c>
@@ -2584,11 +2641,11 @@
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="29" t="s">
+    <row r="101" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B101" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="30"/>
+      <c r="C101" s="12"/>
       <c r="D101" s="9" t="s">
         <v>58</v>
       </c>
@@ -2596,12 +2653,12 @@
       <c r="F101" s="13"/>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="11" t="s">
+    <row r="102" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="103" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B103" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="12"/>
+      <c r="C103" s="18"/>
       <c r="D103" s="9">
         <v>8</v>
       </c>
@@ -2609,11 +2666,11 @@
       <c r="F103" s="13"/>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="11" t="s">
+    <row r="104" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B104" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="12"/>
+      <c r="C104" s="18"/>
       <c r="D104" s="9" t="s">
         <v>73</v>
       </c>
@@ -2621,46 +2678,46 @@
       <c r="F104" s="13"/>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="14" t="s">
+    <row r="105" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B105" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="20"/>
+      <c r="D105" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
-    </row>
-    <row r="106" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="16"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="23" t="s">
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="25"/>
+    </row>
+    <row r="106" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B106" s="21"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="25"/>
-    </row>
-    <row r="107" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="31" t="s">
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="28"/>
+    </row>
+    <row r="107" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B107" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="33"/>
-    </row>
-    <row r="108" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="16"/>
+    </row>
+    <row r="108" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="29" t="s">
+      <c r="C108" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="30"/>
+      <c r="D108" s="12"/>
       <c r="E108" s="2" t="s">
         <v>5</v>
       </c>
@@ -2671,7 +2728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B109" s="3">
         <v>1</v>
       </c>
@@ -2685,7 +2742,7 @@
       <c r="F109" s="4"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B110" s="3">
         <v>2</v>
       </c>
@@ -2699,7 +2756,7 @@
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B111" s="3">
         <v>3</v>
       </c>
@@ -2713,7 +2770,7 @@
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="2:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B112" s="3">
         <v>4</v>
       </c>
@@ -2727,7 +2784,7 @@
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="2:7" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:7" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B113" s="3">
         <v>5</v>
       </c>
@@ -2741,7 +2798,7 @@
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="2:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B114" s="3">
         <v>6</v>
       </c>
@@ -2755,7 +2812,7 @@
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:7" ht="51.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B115" s="3">
         <v>7</v>
       </c>
@@ -2769,11 +2826,11 @@
       <c r="F115" s="4"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="29" t="s">
+    <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B116" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C116" s="30"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="9" t="s">
         <v>90</v>
       </c>
@@ -2781,12 +2838,12 @@
       <c r="F116" s="13"/>
       <c r="G116" s="10"/>
     </row>
-    <row r="117" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="11" t="s">
+    <row r="117" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="118" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B118" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C118" s="12"/>
+      <c r="C118" s="18"/>
       <c r="D118" s="9">
         <v>9</v>
       </c>
@@ -2794,11 +2851,11 @@
       <c r="F118" s="13"/>
       <c r="G118" s="10"/>
     </row>
-    <row r="119" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="11" t="s">
+    <row r="119" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B119" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C119" s="12"/>
+      <c r="C119" s="18"/>
       <c r="D119" s="9" t="s">
         <v>83</v>
       </c>
@@ -2806,46 +2863,46 @@
       <c r="F119" s="13"/>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="14" t="s">
+    <row r="120" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B120" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="15"/>
-      <c r="D120" s="20" t="s">
+      <c r="C120" s="20"/>
+      <c r="D120" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="22"/>
-    </row>
-    <row r="121" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="16"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="23" t="s">
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="25"/>
+    </row>
+    <row r="121" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B121" s="21"/>
+      <c r="C121" s="22"/>
+      <c r="D121" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="25"/>
-    </row>
-    <row r="122" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="31" t="s">
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="28"/>
+    </row>
+    <row r="122" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B122" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="33"/>
-    </row>
-    <row r="123" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="16"/>
+    </row>
+    <row r="123" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="29" t="s">
+      <c r="C123" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="30"/>
+      <c r="D123" s="12"/>
       <c r="E123" s="2" t="s">
         <v>5</v>
       </c>
@@ -2856,7 +2913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B124" s="3">
         <v>1</v>
       </c>
@@ -2874,7 +2931,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B125" s="3">
         <v>2</v>
       </c>
@@ -2892,7 +2949,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="126" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B126" s="3">
         <v>3</v>
       </c>
@@ -2910,7 +2967,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="127" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B127" s="3">
         <v>4</v>
       </c>
@@ -2928,11 +2985,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="128" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="29" t="s">
+    <row r="128" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B128" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="30"/>
+      <c r="C128" s="12"/>
       <c r="D128" s="9" t="s">
         <v>112</v>
       </c>
@@ -2940,12 +2997,12 @@
       <c r="F128" s="13"/>
       <c r="G128" s="10"/>
     </row>
-    <row r="129" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="11" t="s">
+    <row r="129" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="130" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B130" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="12"/>
+      <c r="C130" s="18"/>
       <c r="D130" s="9">
         <v>10</v>
       </c>
@@ -2953,11 +3010,11 @@
       <c r="F130" s="13"/>
       <c r="G130" s="10"/>
     </row>
-    <row r="131" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="11" t="s">
+    <row r="131" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B131" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C131" s="12"/>
+      <c r="C131" s="18"/>
       <c r="D131" s="9" t="s">
         <v>94</v>
       </c>
@@ -2965,46 +3022,46 @@
       <c r="F131" s="13"/>
       <c r="G131" s="10"/>
     </row>
-    <row r="132" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="14" t="s">
+    <row r="132" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B132" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="20" t="s">
+      <c r="C132" s="20"/>
+      <c r="D132" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="22"/>
-    </row>
-    <row r="133" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="16"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="23" t="s">
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="25"/>
+    </row>
+    <row r="133" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B133" s="21"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E133" s="24"/>
-      <c r="F133" s="24"/>
-      <c r="G133" s="25"/>
-    </row>
-    <row r="134" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="31" t="s">
+      <c r="E133" s="27"/>
+      <c r="F133" s="27"/>
+      <c r="G133" s="28"/>
+    </row>
+    <row r="134" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B134" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="32"/>
-      <c r="D134" s="32"/>
-      <c r="E134" s="32"/>
-      <c r="F134" s="32"/>
-      <c r="G134" s="33"/>
-    </row>
-    <row r="135" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="16"/>
+    </row>
+    <row r="135" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="29" t="s">
+      <c r="C135" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="30"/>
+      <c r="D135" s="12"/>
       <c r="E135" s="2" t="s">
         <v>5</v>
       </c>
@@ -3015,7 +3072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B136" s="3">
         <v>1</v>
       </c>
@@ -3033,7 +3090,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="137" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B137" s="3">
         <v>2</v>
       </c>
@@ -3051,7 +3108,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:7" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B138" s="3">
         <v>3</v>
       </c>
@@ -3069,7 +3126,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B139" s="3">
         <v>4</v>
       </c>
@@ -3087,7 +3144,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B140" s="3">
         <v>5</v>
       </c>
@@ -3105,7 +3162,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="141" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B141" s="3">
         <v>6</v>
       </c>
@@ -3123,7 +3180,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="142" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B142" s="3">
         <v>7</v>
       </c>
@@ -3141,7 +3198,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="143" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B143" s="3">
         <v>8</v>
       </c>
@@ -3159,7 +3216,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="144" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B144" s="3">
         <v>9</v>
       </c>
@@ -3177,11 +3234,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="145" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="29" t="s">
+    <row r="145" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B145" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="30"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="9" t="s">
         <v>113</v>
       </c>
@@ -3189,12 +3246,12 @@
       <c r="F145" s="13"/>
       <c r="G145" s="10"/>
     </row>
-    <row r="146" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="147" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="11" t="s">
+    <row r="146" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="147" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B147" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C147" s="12"/>
+      <c r="C147" s="18"/>
       <c r="D147" s="9">
         <v>11</v>
       </c>
@@ -3202,11 +3259,11 @@
       <c r="F147" s="13"/>
       <c r="G147" s="10"/>
     </row>
-    <row r="148" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="11" t="s">
+    <row r="148" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B148" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="12"/>
+      <c r="C148" s="18"/>
       <c r="D148" s="9" t="s">
         <v>124</v>
       </c>
@@ -3214,46 +3271,46 @@
       <c r="F148" s="13"/>
       <c r="G148" s="10"/>
     </row>
-    <row r="149" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="14" t="s">
+    <row r="149" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B149" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C149" s="15"/>
-      <c r="D149" s="20" t="s">
+      <c r="C149" s="20"/>
+      <c r="D149" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="22"/>
-    </row>
-    <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="16"/>
-      <c r="C150" s="17"/>
-      <c r="D150" s="23" t="s">
+      <c r="E149" s="24"/>
+      <c r="F149" s="24"/>
+      <c r="G149" s="25"/>
+    </row>
+    <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B150" s="21"/>
+      <c r="C150" s="22"/>
+      <c r="D150" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E150" s="24"/>
-      <c r="F150" s="24"/>
-      <c r="G150" s="25"/>
-    </row>
-    <row r="151" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="31" t="s">
+      <c r="E150" s="27"/>
+      <c r="F150" s="27"/>
+      <c r="G150" s="28"/>
+    </row>
+    <row r="151" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B151" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C151" s="32"/>
-      <c r="D151" s="32"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="32"/>
-      <c r="G151" s="33"/>
-    </row>
-    <row r="152" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="15"/>
+      <c r="D151" s="15"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="16"/>
+    </row>
+    <row r="152" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B152" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C152" s="29" t="s">
+      <c r="C152" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D152" s="30"/>
+      <c r="D152" s="12"/>
       <c r="E152" s="2" t="s">
         <v>5</v>
       </c>
@@ -3264,7 +3321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B153" s="3">
         <v>1</v>
       </c>
@@ -3282,7 +3339,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="154" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B154" s="3">
         <v>2</v>
       </c>
@@ -3300,7 +3357,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="155" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B155" s="3">
         <v>3</v>
       </c>
@@ -3318,7 +3375,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="156" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B156" s="3">
         <v>4</v>
       </c>
@@ -3336,7 +3393,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="157" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B157" s="3">
         <v>5</v>
       </c>
@@ -3354,7 +3411,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="158" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B158" s="3">
         <v>6</v>
       </c>
@@ -3372,11 +3429,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="159" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="29" t="s">
+    <row r="159" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B159" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C159" s="30"/>
+      <c r="C159" s="12"/>
       <c r="D159" s="9" t="s">
         <v>135</v>
       </c>
@@ -3384,12 +3441,12 @@
       <c r="F159" s="13"/>
       <c r="G159" s="10"/>
     </row>
-    <row r="160" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="11" t="s">
+    <row r="160" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="161" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B161" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="12"/>
+      <c r="C161" s="18"/>
       <c r="D161" s="9">
         <v>12</v>
       </c>
@@ -3397,11 +3454,11 @@
       <c r="F161" s="13"/>
       <c r="G161" s="10"/>
     </row>
-    <row r="162" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="11" t="s">
+    <row r="162" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B162" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="12"/>
+      <c r="C162" s="18"/>
       <c r="D162" s="9" t="s">
         <v>114</v>
       </c>
@@ -3409,46 +3466,46 @@
       <c r="F162" s="13"/>
       <c r="G162" s="10"/>
     </row>
-    <row r="163" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="14" t="s">
+    <row r="163" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B163" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C163" s="15"/>
-      <c r="D163" s="20" t="s">
+      <c r="C163" s="20"/>
+      <c r="D163" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="22"/>
-    </row>
-    <row r="164" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="16"/>
-      <c r="C164" s="17"/>
-      <c r="D164" s="23" t="s">
+      <c r="E163" s="24"/>
+      <c r="F163" s="24"/>
+      <c r="G163" s="25"/>
+    </row>
+    <row r="164" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B164" s="21"/>
+      <c r="C164" s="22"/>
+      <c r="D164" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="E164" s="24"/>
-      <c r="F164" s="24"/>
-      <c r="G164" s="25"/>
-    </row>
-    <row r="165" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="31" t="s">
+      <c r="E164" s="27"/>
+      <c r="F164" s="27"/>
+      <c r="G164" s="28"/>
+    </row>
+    <row r="165" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B165" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="32"/>
-      <c r="D165" s="32"/>
-      <c r="E165" s="32"/>
-      <c r="F165" s="32"/>
-      <c r="G165" s="33"/>
-    </row>
-    <row r="166" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="15"/>
+      <c r="D165" s="15"/>
+      <c r="E165" s="15"/>
+      <c r="F165" s="15"/>
+      <c r="G165" s="16"/>
+    </row>
+    <row r="166" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B166" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C166" s="29" t="s">
+      <c r="C166" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="30"/>
+      <c r="D166" s="12"/>
       <c r="E166" s="2" t="s">
         <v>5</v>
       </c>
@@ -3459,7 +3516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B167" s="3">
         <v>1</v>
       </c>
@@ -3477,7 +3534,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="168" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B168" s="3">
         <v>2</v>
       </c>
@@ -3495,7 +3552,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="169" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:7" ht="26.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B169" s="3">
         <v>3</v>
       </c>
@@ -3513,7 +3570,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="170" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B170" s="3">
         <v>4</v>
       </c>
@@ -3531,7 +3588,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="171" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B171" s="3">
         <v>5</v>
       </c>
@@ -3549,11 +3606,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="172" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="29" t="s">
+    <row r="172" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B172" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C172" s="30"/>
+      <c r="C172" s="12"/>
       <c r="D172" s="9" t="s">
         <v>123</v>
       </c>
@@ -3561,9 +3618,193 @@
       <c r="F172" s="13"/>
       <c r="G172" s="10"/>
     </row>
-    <row r="173" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="D172:G172"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:G162"/>
+    <mergeCell ref="B163:C164"/>
+    <mergeCell ref="D163:G163"/>
+    <mergeCell ref="D164:G164"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="D159:G159"/>
+    <mergeCell ref="B151:G151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:G147"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="B149:C150"/>
+    <mergeCell ref="D149:G149"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:G128"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:G130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:G131"/>
+    <mergeCell ref="B132:C133"/>
+    <mergeCell ref="D132:G132"/>
+    <mergeCell ref="D133:G133"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C121"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="B122:G122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:G118"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="B74:C75"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:G89"/>
+    <mergeCell ref="B90:C91"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D91:G91"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:G88"/>
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="B116:C116"/>
     <mergeCell ref="D116:G116"/>
@@ -3588,51 +3829,764 @@
     <mergeCell ref="C93:D93"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:G89"/>
-    <mergeCell ref="B90:C91"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D91:G91"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="B74:C75"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="D75:G75"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E192BF06-66C7-4B4F-95C1-D1A93166083F}">
+  <dimension ref="B4:G58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="3" max="3" width="32.59765625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="35.265625" customWidth="1"/>
+    <col min="6" max="6" width="33.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="9">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="3">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" s="10"/>
+      <c r="E16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="19" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="9">
+        <v>10</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="18"/>
+      <c r="D20" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B23" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="45.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B26" s="3">
+        <v>2</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="29.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B30" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="32" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B32" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="9">
+        <v>11</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="18"/>
+      <c r="D33" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
+    </row>
+    <row r="35" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25"/>
+    </row>
+    <row r="36" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B37" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="10"/>
+      <c r="E39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D40" s="10"/>
+      <c r="E40" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="39.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D41" s="10"/>
+      <c r="E41" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="40.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B42" s="3">
+        <v>4</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B43" s="3">
+        <v>5</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43" s="10"/>
+      <c r="E43" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="46" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B46" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="9">
+        <v>12</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B47" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B48" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="20"/>
+      <c r="D48" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="25"/>
+    </row>
+    <row r="49" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="25"/>
+    </row>
+    <row r="50" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="28"/>
+    </row>
+    <row r="51" spans="2:7" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B51" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="16"/>
+    </row>
+    <row r="52" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="30.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B53" s="3">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D53" s="10"/>
+      <c r="E53" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B54" s="3">
+        <v>2</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="E54" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B55" s="3">
+        <v>3</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="D55" s="10"/>
+      <c r="E55" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="54.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B56" s="3">
+        <v>4</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D56" s="10"/>
+      <c r="E56" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="2:7" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <mergeCells count="66">
     <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:G57"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="C52:D52"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="C55:D55"/>
@@ -3640,555 +4594,27 @@
     <mergeCell ref="D46:G46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="D47:G47"/>
-    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="B48:C50"/>
     <mergeCell ref="D48:G48"/>
     <mergeCell ref="D49:G49"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="D50:G50"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="C43:D43"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B34:C36"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="B37:G37"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:G118"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C121"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="B122:G122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="B149:C150"/>
-    <mergeCell ref="D149:G149"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:G128"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D130:G130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="D131:G131"/>
-    <mergeCell ref="B132:C133"/>
-    <mergeCell ref="D132:G132"/>
-    <mergeCell ref="D133:G133"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="D159:G159"/>
-    <mergeCell ref="B151:G151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="D147:G147"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="D172:G172"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="D162:G162"/>
-    <mergeCell ref="B163:C164"/>
-    <mergeCell ref="D163:G163"/>
-    <mergeCell ref="D164:G164"/>
-    <mergeCell ref="B165:G165"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="C41:D41"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="D33:G33"/>
     <mergeCell ref="D34:G34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:C29"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E192BF06-66C7-4B4F-95C1-D1A93166083F}">
-  <dimension ref="B4:G31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="9">
-        <v>8</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10"/>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-    </row>
-    <row r="10" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>3</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <v>4</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <v>6</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="9">
-        <v>9</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="45.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="3">
-        <v>2</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="3">
-        <v>3</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="29.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="3">
-        <v>4</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="3">
-        <v>5</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="D36:G36"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
@@ -4202,6 +4628,26 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2 test cases for Animax in Selenium and updated excel
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csd\Desktop\products\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roxy Enescu\Desktop\SoftwareApplicationTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D4128DB-3984-4398-B733-45B1C1BFEEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89D5F57-BBE3-4A60-A197-B025CFE1A381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Testarea funcțională" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="199">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -100,15 +100,9 @@
     <t>Se afișează un formular cu informațiile curente ale utilizatorului</t>
   </si>
   <si>
-    <t>Se modifică detaliile dorite (prenume și număr de telefon)</t>
-  </si>
-  <si>
     <t>Câmpurile pot fi editate</t>
   </si>
   <si>
-    <t>Se salvează modificările</t>
-  </si>
-  <si>
     <t>Modificările sunt salvate și se afișează un mesaj de confirmare</t>
   </si>
   <si>
@@ -250,9 +244,6 @@
     <t>Zooplus - Aplicare reducere 5% după abonarea la newsletter</t>
   </si>
   <si>
-    <t>Se accesează coșul de cumpărături prin butonul "Coș"</t>
-  </si>
-  <si>
     <t>Se accesează secțiunea "Contul Meu"</t>
   </si>
   <si>
@@ -623,6 +614,15 @@
   </si>
   <si>
     <t>Voucherul aferent produsului este selectat</t>
+  </si>
+  <si>
+    <t>Se accesează coșul de cumpărături prin butonul "VEZI COSUL DE CUMPARATURI"</t>
+  </si>
+  <si>
+    <t>Se modifică detaliile dorite (Prenume)</t>
+  </si>
+  <si>
+    <t>Se salvează modificările apăsând butonul "Trimite"</t>
   </si>
 </sst>
 </file>
@@ -944,13 +944,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -962,12 +977,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -988,6 +997,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -995,21 +1010,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1295,26 +1295,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:G47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="9">
         <v>1</v>
       </c>
@@ -1322,58 +1322,58 @@
       <c r="F2" s="13"/>
       <c r="G2" s="10"/>
     </row>
-    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+    <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
-    </row>
-    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="23" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1384,49 +1384,61 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>1</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>4</v>
       </c>
@@ -1437,10 +1449,14 @@
       <c r="E11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>5</v>
       </c>
@@ -1451,28 +1467,36 @@
       <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>6</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="29" t="s">
+      <c r="F13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1480,12 +1504,12 @@
       <c r="F14" s="13"/>
       <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
+    <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="9">
         <v>2</v>
       </c>
@@ -1493,68 +1517,68 @@
       <c r="F16" s="13"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
+    <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23" t="s">
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-    </row>
-    <row r="21" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="31" t="s">
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
+    </row>
+    <row r="21" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-    </row>
-    <row r="22" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1565,108 +1589,132 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>1</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>2</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
-    </row>
-    <row r="25" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>3</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-    </row>
-    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>4</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>24</v>
+        <v>197</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>5</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>26</v>
+        <v>198</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="5"/>
-    </row>
-    <row r="28" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>6</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="11" t="s">
+    <row r="30" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="9">
         <v>3</v>
       </c>
@@ -1674,58 +1722,58 @@
       <c r="F31" s="13"/>
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11" t="s">
+    <row r="32" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="20" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
-    </row>
-    <row r="34" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="23" t="s">
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
+    </row>
+    <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-    </row>
-    <row r="35" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="31" t="s">
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-    </row>
-    <row r="36" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1736,12 +1784,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="3">
         <v>1</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D37" s="10"/>
       <c r="E37" s="4" t="s">
@@ -1751,135 +1799,135 @@
         <v>12</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="3">
         <v>2</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D38" s="10"/>
       <c r="E38" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="3">
         <v>3</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="3">
         <v>4</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="3">
         <v>5</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="3">
         <v>6</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="3">
         <v>7</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D43" s="10"/>
       <c r="E43" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E44" s="13"/>
       <c r="F44" s="13"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="11" t="s">
+    <row r="45" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="9">
         <v>4</v>
       </c>
@@ -1887,58 +1935,58 @@
       <c r="F46" s="13"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
+    <row r="47" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="14" t="s">
+    <row r="48" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="20" t="s">
+      <c r="C48" s="20"/>
+      <c r="D48" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="16"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="23" t="s">
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="25"/>
+    </row>
+    <row r="49" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
-    </row>
-    <row r="50" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="31" t="s">
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="28"/>
+    </row>
+    <row r="50" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
-    </row>
-    <row r="51" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="16"/>
+    </row>
+    <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="2" t="s">
         <v>5</v>
       </c>
@@ -1949,12 +1997,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="3">
         <v>1</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="4" t="s">
@@ -1964,117 +2012,117 @@
         <v>12</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="3">
         <v>2</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="3">
         <v>3</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="3">
         <v>4</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="3">
         <v>5</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D56" s="10"/>
       <c r="E56" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="57" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B57" s="3">
         <v>6</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="30"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E58" s="13"/>
       <c r="F58" s="13"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="11" t="s">
+    <row r="59" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="18"/>
       <c r="D60" s="9">
         <v>5</v>
       </c>
@@ -2082,58 +2130,58 @@
       <c r="F60" s="13"/>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="11" t="s">
+    <row r="61" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="12"/>
+      <c r="C61" s="18"/>
       <c r="D61" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="14" t="s">
+    <row r="62" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="20"/>
+      <c r="D62" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22"/>
-    </row>
-    <row r="63" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="16"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
-    </row>
-    <row r="64" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="31" t="s">
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
+    </row>
+    <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="28"/>
+    </row>
+    <row r="64" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
-    </row>
-    <row r="65" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="16"/>
+    </row>
+    <row r="65" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="30"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2144,80 +2192,80 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B66" s="3">
         <v>1</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D66" s="10"/>
       <c r="E66" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="5"/>
     </row>
-    <row r="67" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="3">
         <v>2</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D67" s="10"/>
       <c r="E67" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="5"/>
     </row>
-    <row r="68" spans="2:7" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:7" ht="34.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="3">
         <v>3</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D68" s="10"/>
       <c r="E68" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="5"/>
     </row>
-    <row r="69" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B69" s="3">
         <v>4</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D69" s="10"/>
       <c r="E69" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="5"/>
     </row>
-    <row r="70" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="29" t="s">
+    <row r="70" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="30"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E70" s="13"/>
       <c r="F70" s="13"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="11" t="s">
+    <row r="71" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="12"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="9">
         <v>6</v>
       </c>
@@ -2225,58 +2273,58 @@
       <c r="F72" s="13"/>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="11" t="s">
+    <row r="73" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="12"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13"/>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
+    <row r="74" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="20"/>
+      <c r="D74" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="22"/>
-    </row>
-    <row r="75" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="16"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
-    </row>
-    <row r="76" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="31" t="s">
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="25"/>
+    </row>
+    <row r="75" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="28"/>
+    </row>
+    <row r="76" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33"/>
-    </row>
-    <row r="77" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="16"/>
+    </row>
+    <row r="77" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="30"/>
+      <c r="D77" s="12"/>
       <c r="E77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2287,77 +2335,77 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="3">
         <v>1</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D78" s="10"/>
       <c r="E78" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F78" s="4"/>
       <c r="G78" s="5"/>
     </row>
-    <row r="79" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="3">
         <v>2</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D79" s="10"/>
       <c r="E79" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F79" s="4"/>
       <c r="G79" s="5"/>
     </row>
-    <row r="80" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="3">
         <v>3</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D80" s="10"/>
       <c r="E80" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F80" s="4"/>
       <c r="G80" s="5"/>
     </row>
-    <row r="81" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B81" s="3">
         <v>4</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D81" s="10"/>
       <c r="E81" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F81" s="4"/>
       <c r="G81" s="5"/>
     </row>
-    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B82" s="3">
         <v>5</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D82" s="10"/>
       <c r="E82" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="5"/>
     </row>
-    <row r="83" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B83" s="3">
         <v>6</v>
       </c>
@@ -2371,52 +2419,52 @@
       <c r="F83" s="4"/>
       <c r="G83" s="5"/>
     </row>
-    <row r="84" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B84" s="3">
         <v>7</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D84" s="10"/>
       <c r="E84" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F84" s="4"/>
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="2:7" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="3">
         <v>8</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D85" s="10"/>
       <c r="E85" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="29" t="s">
+    <row r="86" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="30"/>
+      <c r="C86" s="12"/>
       <c r="D86" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E86" s="13"/>
       <c r="F86" s="13"/>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="11" t="s">
+    <row r="87" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="12"/>
+      <c r="C88" s="18"/>
       <c r="D88" s="9">
         <v>7</v>
       </c>
@@ -2424,58 +2472,58 @@
       <c r="F88" s="13"/>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="11" t="s">
+    <row r="89" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="12"/>
+      <c r="C89" s="18"/>
       <c r="D89" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E89" s="13"/>
       <c r="F89" s="13"/>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="14" t="s">
+    <row r="90" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20" t="s">
+      <c r="C90" s="20"/>
+      <c r="D90" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="22"/>
-    </row>
-    <row r="91" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="16"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
-    </row>
-    <row r="92" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="31" t="s">
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
+    </row>
+    <row r="91" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="28"/>
+    </row>
+    <row r="92" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
-    </row>
-    <row r="93" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="16"/>
+    </row>
+    <row r="93" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="29" t="s">
+      <c r="C93" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="30"/>
+      <c r="D93" s="12"/>
       <c r="E93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2486,122 +2534,122 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="3">
         <v>1</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D94" s="10"/>
       <c r="E94" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F94" s="4"/>
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="3">
         <v>2</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D95" s="10"/>
       <c r="E95" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F95" s="4"/>
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="2:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B96" s="3">
         <v>3</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D96" s="10"/>
       <c r="E96" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F96" s="4"/>
       <c r="G96" s="5"/>
     </row>
-    <row r="97" spans="2:7" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7" ht="51" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B97" s="3">
         <v>4</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D97" s="10"/>
       <c r="E97" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F97" s="4"/>
       <c r="G97" s="5"/>
     </row>
-    <row r="98" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B98" s="3">
         <v>5</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D98" s="10"/>
       <c r="E98" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F98" s="4"/>
       <c r="G98" s="5"/>
     </row>
-    <row r="99" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B99" s="3">
         <v>6</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D99" s="10"/>
       <c r="E99" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F99" s="4"/>
       <c r="G99" s="5"/>
     </row>
-    <row r="100" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="3">
         <v>7</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D100" s="10"/>
       <c r="E100" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F100" s="4"/>
       <c r="G100" s="5"/>
     </row>
-    <row r="101" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="29" t="s">
+    <row r="101" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="30"/>
+      <c r="C101" s="12"/>
       <c r="D101" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E101" s="13"/>
       <c r="F101" s="13"/>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="11" t="s">
+    <row r="102" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="12"/>
+      <c r="C103" s="18"/>
       <c r="D103" s="9">
         <v>8</v>
       </c>
@@ -2609,58 +2657,58 @@
       <c r="F103" s="13"/>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="11" t="s">
+    <row r="104" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="12"/>
+      <c r="C104" s="18"/>
       <c r="D104" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E104" s="13"/>
       <c r="F104" s="13"/>
       <c r="G104" s="10"/>
     </row>
-    <row r="105" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="14" t="s">
+    <row r="105" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B105" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="20"/>
+      <c r="D105" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
-    </row>
-    <row r="106" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="16"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="25"/>
-    </row>
-    <row r="107" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="31" t="s">
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="25"/>
+    </row>
+    <row r="106" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="21"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="28"/>
+    </row>
+    <row r="107" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="33"/>
-    </row>
-    <row r="108" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="16"/>
+    </row>
+    <row r="108" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="29" t="s">
+      <c r="C108" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="30"/>
+      <c r="D108" s="12"/>
       <c r="E108" s="2" t="s">
         <v>5</v>
       </c>
@@ -2671,122 +2719,122 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B109" s="3">
         <v>1</v>
       </c>
       <c r="C109" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F109" s="4"/>
       <c r="G109" s="5"/>
     </row>
-    <row r="110" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="3">
         <v>2</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F110" s="4"/>
       <c r="G110" s="5"/>
     </row>
-    <row r="111" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B111" s="3">
         <v>3</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D111" s="10"/>
       <c r="E111" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F111" s="4"/>
       <c r="G111" s="5"/>
     </row>
-    <row r="112" spans="2:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:7" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="3">
         <v>4</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D112" s="10"/>
       <c r="E112" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F112" s="4"/>
       <c r="G112" s="5"/>
     </row>
-    <row r="113" spans="2:7" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:7" ht="57" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B113" s="3">
         <v>5</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D113" s="10"/>
       <c r="E113" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F113" s="4"/>
       <c r="G113" s="5"/>
     </row>
-    <row r="114" spans="2:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:7" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="3">
         <v>6</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D114" s="10"/>
       <c r="E114" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F114" s="4"/>
       <c r="G114" s="5"/>
     </row>
-    <row r="115" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:7" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="3">
         <v>7</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D115" s="10"/>
       <c r="E115" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F115" s="4"/>
       <c r="G115" s="5"/>
     </row>
-    <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B116" s="29" t="s">
+    <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C116" s="30"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13"/>
       <c r="G116" s="10"/>
     </row>
-    <row r="117" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B118" s="11" t="s">
+    <row r="117" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B118" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C118" s="12"/>
+      <c r="C118" s="18"/>
       <c r="D118" s="9">
         <v>9</v>
       </c>
@@ -2794,58 +2842,58 @@
       <c r="F118" s="13"/>
       <c r="G118" s="10"/>
     </row>
-    <row r="119" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B119" s="11" t="s">
+    <row r="119" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C119" s="12"/>
+      <c r="C119" s="18"/>
       <c r="D119" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="13"/>
       <c r="G119" s="10"/>
     </row>
-    <row r="120" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="14" t="s">
+    <row r="120" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B120" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="15"/>
-      <c r="D120" s="20" t="s">
+      <c r="C120" s="20"/>
+      <c r="D120" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="22"/>
-    </row>
-    <row r="121" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="16"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="25"/>
-    </row>
-    <row r="122" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B122" s="31" t="s">
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="25"/>
+    </row>
+    <row r="121" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="21"/>
+      <c r="C121" s="22"/>
+      <c r="D121" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="28"/>
+    </row>
+    <row r="122" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B122" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="33"/>
-    </row>
-    <row r="123" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="16"/>
+    </row>
+    <row r="123" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="29" t="s">
+      <c r="C123" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="30"/>
+      <c r="D123" s="12"/>
       <c r="E123" s="2" t="s">
         <v>5</v>
       </c>
@@ -2856,96 +2904,96 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B124" s="3">
         <v>1</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G124" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="3">
         <v>2</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D125" s="10"/>
       <c r="E125" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="3">
         <v>3</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G126" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" ht="44.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B127" s="3">
         <v>4</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G127" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B128" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B128" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="30"/>
+      <c r="C128" s="12"/>
       <c r="D128" s="9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E128" s="13"/>
       <c r="F128" s="13"/>
       <c r="G128" s="10"/>
     </row>
-    <row r="129" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="130" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B130" s="11" t="s">
+    <row r="129" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="130" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B130" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="12"/>
+      <c r="C130" s="18"/>
       <c r="D130" s="9">
         <v>10</v>
       </c>
@@ -2953,58 +3001,58 @@
       <c r="F130" s="13"/>
       <c r="G130" s="10"/>
     </row>
-    <row r="131" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="11" t="s">
+    <row r="131" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B131" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C131" s="12"/>
+      <c r="C131" s="18"/>
       <c r="D131" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E131" s="13"/>
       <c r="F131" s="13"/>
       <c r="G131" s="10"/>
     </row>
-    <row r="132" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="14" t="s">
+    <row r="132" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="20" t="s">
+      <c r="C132" s="20"/>
+      <c r="D132" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="22"/>
-    </row>
-    <row r="133" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B133" s="16"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E133" s="24"/>
-      <c r="F133" s="24"/>
-      <c r="G133" s="25"/>
-    </row>
-    <row r="134" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B134" s="31" t="s">
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="25"/>
+    </row>
+    <row r="133" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B133" s="21"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E133" s="27"/>
+      <c r="F133" s="27"/>
+      <c r="G133" s="28"/>
+    </row>
+    <row r="134" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B134" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="32"/>
-      <c r="D134" s="32"/>
-      <c r="E134" s="32"/>
-      <c r="F134" s="32"/>
-      <c r="G134" s="33"/>
-    </row>
-    <row r="135" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="16"/>
+    </row>
+    <row r="135" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="29" t="s">
+      <c r="C135" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="30"/>
+      <c r="D135" s="12"/>
       <c r="E135" s="2" t="s">
         <v>5</v>
       </c>
@@ -3015,186 +3063,186 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="3">
         <v>1</v>
       </c>
       <c r="C136" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D136" s="10"/>
       <c r="E136" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F136" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G136" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="3">
         <v>2</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D137" s="10"/>
       <c r="E137" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F137" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G137" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="138" spans="2:7" ht="65.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B138" s="3">
         <v>3</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D138" s="10"/>
       <c r="E138" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F138" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G138" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B139" s="3">
         <v>4</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D139" s="10"/>
       <c r="E139" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F139" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G139" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="140" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="3">
         <v>5</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D140" s="10"/>
       <c r="E140" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G140" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="3">
         <v>6</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D141" s="10"/>
       <c r="E141" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G141" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="3">
         <v>7</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D142" s="10"/>
       <c r="E142" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F142" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G142" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="3">
         <v>8</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D143" s="10"/>
       <c r="E143" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G143" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" ht="38.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B144" s="3">
         <v>9</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D144" s="10"/>
       <c r="E144" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F144" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G144" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B145" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B145" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="30"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E145" s="13"/>
       <c r="F145" s="13"/>
       <c r="G145" s="10"/>
     </row>
-    <row r="146" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="147" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B147" s="11" t="s">
+    <row r="146" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="147" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B147" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C147" s="12"/>
+      <c r="C147" s="18"/>
       <c r="D147" s="9">
         <v>11</v>
       </c>
@@ -3202,58 +3250,58 @@
       <c r="F147" s="13"/>
       <c r="G147" s="10"/>
     </row>
-    <row r="148" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B148" s="11" t="s">
+    <row r="148" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="12"/>
+      <c r="C148" s="18"/>
       <c r="D148" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E148" s="13"/>
       <c r="F148" s="13"/>
       <c r="G148" s="10"/>
     </row>
-    <row r="149" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B149" s="14" t="s">
+    <row r="149" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B149" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C149" s="15"/>
-      <c r="D149" s="20" t="s">
+      <c r="C149" s="20"/>
+      <c r="D149" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="22"/>
-    </row>
-    <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B150" s="16"/>
-      <c r="C150" s="17"/>
-      <c r="D150" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E150" s="24"/>
-      <c r="F150" s="24"/>
-      <c r="G150" s="25"/>
-    </row>
-    <row r="151" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B151" s="31" t="s">
+      <c r="E149" s="24"/>
+      <c r="F149" s="24"/>
+      <c r="G149" s="25"/>
+    </row>
+    <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B150" s="21"/>
+      <c r="C150" s="22"/>
+      <c r="D150" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E150" s="27"/>
+      <c r="F150" s="27"/>
+      <c r="G150" s="28"/>
+    </row>
+    <row r="151" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B151" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C151" s="32"/>
-      <c r="D151" s="32"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="32"/>
-      <c r="G151" s="33"/>
-    </row>
-    <row r="152" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C151" s="15"/>
+      <c r="D151" s="15"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="16"/>
+    </row>
+    <row r="152" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C152" s="29" t="s">
+      <c r="C152" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D152" s="30"/>
+      <c r="D152" s="12"/>
       <c r="E152" s="2" t="s">
         <v>5</v>
       </c>
@@ -3264,132 +3312,132 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B153" s="3">
         <v>1</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D153" s="10"/>
       <c r="E153" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F153" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G153" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" ht="52.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B154" s="3">
         <v>2</v>
       </c>
       <c r="C154" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D154" s="10"/>
       <c r="E154" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B155" s="3">
         <v>3</v>
       </c>
       <c r="C155" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D155" s="10"/>
       <c r="E155" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F155" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G155" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="3">
         <v>4</v>
       </c>
       <c r="C156" s="9" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D156" s="10"/>
       <c r="E156" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F156" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G156" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="3">
         <v>5</v>
       </c>
       <c r="C157" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D157" s="10"/>
       <c r="E157" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G157" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="3">
         <v>6</v>
       </c>
       <c r="C158" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D158" s="10"/>
       <c r="E158" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F158" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G158" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B159" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B159" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C159" s="30"/>
+      <c r="C159" s="12"/>
       <c r="D159" s="9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E159" s="13"/>
       <c r="F159" s="13"/>
       <c r="G159" s="10"/>
     </row>
-    <row r="160" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="161" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B161" s="11" t="s">
+    <row r="160" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="161" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B161" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="12"/>
+      <c r="C161" s="18"/>
       <c r="D161" s="9">
         <v>12</v>
       </c>
@@ -3397,58 +3445,58 @@
       <c r="F161" s="13"/>
       <c r="G161" s="10"/>
     </row>
-    <row r="162" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B162" s="11" t="s">
+    <row r="162" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B162" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="12"/>
+      <c r="C162" s="18"/>
       <c r="D162" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E162" s="13"/>
       <c r="F162" s="13"/>
       <c r="G162" s="10"/>
     </row>
-    <row r="163" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B163" s="14" t="s">
+    <row r="163" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B163" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C163" s="15"/>
-      <c r="D163" s="20" t="s">
+      <c r="C163" s="20"/>
+      <c r="D163" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="22"/>
-    </row>
-    <row r="164" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B164" s="16"/>
-      <c r="C164" s="17"/>
-      <c r="D164" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E164" s="24"/>
-      <c r="F164" s="24"/>
-      <c r="G164" s="25"/>
-    </row>
-    <row r="165" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B165" s="31" t="s">
+      <c r="E163" s="24"/>
+      <c r="F163" s="24"/>
+      <c r="G163" s="25"/>
+    </row>
+    <row r="164" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B164" s="21"/>
+      <c r="C164" s="22"/>
+      <c r="D164" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E164" s="27"/>
+      <c r="F164" s="27"/>
+      <c r="G164" s="28"/>
+    </row>
+    <row r="165" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B165" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="32"/>
-      <c r="D165" s="32"/>
-      <c r="E165" s="32"/>
-      <c r="F165" s="32"/>
-      <c r="G165" s="33"/>
-    </row>
-    <row r="166" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C165" s="15"/>
+      <c r="D165" s="15"/>
+      <c r="E165" s="15"/>
+      <c r="F165" s="15"/>
+      <c r="G165" s="16"/>
+    </row>
+    <row r="166" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C166" s="29" t="s">
+      <c r="C166" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="30"/>
+      <c r="D166" s="12"/>
       <c r="E166" s="2" t="s">
         <v>5</v>
       </c>
@@ -3459,111 +3507,295 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B167" s="3">
         <v>1</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D167" s="10"/>
       <c r="E167" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F167" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="168" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B168" s="3">
         <v>2</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D168" s="10"/>
       <c r="E168" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F168" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="169" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B169" s="3">
         <v>3</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D169" s="10"/>
       <c r="E169" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F169" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G169" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="170" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B170" s="3">
         <v>4</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D170" s="10"/>
       <c r="E170" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F170" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="171" spans="2:7" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B171" s="3">
         <v>5</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D171" s="10"/>
       <c r="E171" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G171" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="172" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B172" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B172" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C172" s="30"/>
+      <c r="C172" s="12"/>
       <c r="D172" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E172" s="13"/>
       <c r="F172" s="13"/>
       <c r="G172" s="10"/>
     </row>
-    <row r="173" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="D172:G172"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:G162"/>
+    <mergeCell ref="B163:C164"/>
+    <mergeCell ref="D163:G163"/>
+    <mergeCell ref="D164:G164"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="D159:G159"/>
+    <mergeCell ref="B151:G151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:G147"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="B149:C150"/>
+    <mergeCell ref="D149:G149"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:G128"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:G130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:G131"/>
+    <mergeCell ref="B132:C133"/>
+    <mergeCell ref="D132:G132"/>
+    <mergeCell ref="D133:G133"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C121"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="B122:G122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:G118"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="B74:C75"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:G89"/>
+    <mergeCell ref="B90:C91"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D91:G91"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:G88"/>
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="B116:C116"/>
     <mergeCell ref="D116:G116"/>
@@ -3588,190 +3820,6 @@
     <mergeCell ref="C93:D93"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:G89"/>
-    <mergeCell ref="B90:C91"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D91:G91"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="B74:C75"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="D75:G75"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:G118"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C121"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="B122:G122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="B149:C150"/>
-    <mergeCell ref="D149:G149"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:G128"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D130:G130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="D131:G131"/>
-    <mergeCell ref="B132:C133"/>
-    <mergeCell ref="D132:G132"/>
-    <mergeCell ref="D133:G133"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="D159:G159"/>
-    <mergeCell ref="B151:G151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="D147:G147"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="D172:G172"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="D162:G162"/>
-    <mergeCell ref="B163:C164"/>
-    <mergeCell ref="D163:G163"/>
-    <mergeCell ref="D164:G164"/>
-    <mergeCell ref="B165:G165"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:C34"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3785,21 +3833,21 @@
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="32.5546875" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="9">
         <v>8</v>
       </c>
@@ -3807,58 +3855,58 @@
       <c r="F5" s="13"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
-    </row>
-    <row r="10" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="30"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
@@ -3869,132 +3917,132 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="37.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="37.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="43.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>5</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="34.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="34.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>6</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="30"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+    <row r="18" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="18"/>
       <c r="D19" s="9">
         <v>9</v>
       </c>
@@ -4002,58 +4050,58 @@
       <c r="F19" s="13"/>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+    <row r="20" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+    <row r="21" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="20" t="s">
+      <c r="C21" s="20"/>
+      <c r="D21" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="31" t="s">
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="25"/>
+    </row>
+    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="21"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" spans="2:7" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="2" t="s">
         <v>5</v>
       </c>
@@ -4064,131 +4112,111 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="45.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:7" ht="45.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="37.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="37.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>2</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>3</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="29.65" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="29.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>4</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="31.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="31.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>5</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="30"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="9" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:G5"/>
@@ -4202,6 +4230,26 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:G21"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 4 test cases in excel for performance testing Animax
</commit_message>
<xml_diff>
--- a/Cazuri de testare.xlsx
+++ b/Cazuri de testare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roxy Enescu\Desktop\SoftwareApplicationTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECAA1F1-7E13-4EC9-AC8F-DA033F7307B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A293033-D992-4B58-B155-8AFAC2D29EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="250">
   <si>
     <t>Summary / Title</t>
   </si>
@@ -680,6 +680,102 @@
   </si>
   <si>
     <t>Lista afișată reflectă atât textul din căutare cât și filtrele selectate</t>
+  </si>
+  <si>
+    <t>Animax - Verificarea navigării de la o pagină la alta</t>
+  </si>
+  <si>
+    <t>Se accesează pagina "https://animax.ro/"</t>
+  </si>
+  <si>
+    <t>Se afișează lista de produse din subcategoria "Hrană umedă"</t>
+  </si>
+  <si>
+    <t>Se navighează la subcategoria "Hrană umedă"</t>
+  </si>
+  <si>
+    <t>Se apasă butonul "Următorul" din josul paginii de produse</t>
+  </si>
+  <si>
+    <t>Se afișează lista de pe pagina 2 de produse din subcategoria "Hrană umedă"</t>
+  </si>
+  <si>
+    <t>Lista afișată reflectă produsele de pe pagina a doua a categoriei.</t>
+  </si>
+  <si>
+    <t>Verificarea filtrării și sortării produselor dintr-o anumită categorie</t>
+  </si>
+  <si>
+    <t>Se sortează lista de produse după "Cel mai bine vândut"</t>
+  </si>
+  <si>
+    <t>Se filtrează lista după preț (între 9 și 15 lei)</t>
+  </si>
+  <si>
+    <t>Se afișează lista de produse din subcategoria "Hrană umedă" în funcție de cel mai bine vândut produs</t>
+  </si>
+  <si>
+    <t>Se afișează lista de produse din subcategoria "Hrană umedă" cu prețurile în intervalul 9-15 lei.</t>
+  </si>
+  <si>
+    <t>Lista de produse afișată este sortată după cel mai bine vândut și după prețul dat.</t>
+  </si>
+  <si>
+    <t>Se navighează la categoria "Jucării"</t>
+  </si>
+  <si>
+    <t>Se selectează o subcategorie aleatorie</t>
+  </si>
+  <si>
+    <t>Se afișează lista de produse din subcategoria aleasă</t>
+  </si>
+  <si>
+    <t>Se selectează un produs aleatoriu</t>
+  </si>
+  <si>
+    <t>Se afișează pagina de detalii a produsului selectat</t>
+  </si>
+  <si>
+    <t>Se măsoară timpul de încărcare al paginii de detalii</t>
+  </si>
+  <si>
+    <t>Pagina de detalii se încarcă într-un timp satisfăcător (de exemplu, sub 3 secunde)</t>
+  </si>
+  <si>
+    <t>Pagina de detalii produs se încarcă eficient și în limitele de performanță stabilite.</t>
+  </si>
+  <si>
+    <t>Verificarea timpului de încărcare pentru paginile de detalii ale produselor</t>
+  </si>
+  <si>
+    <t>Evaluarea performanței și a stabilității sistemului de autentificare sub încărcare</t>
+  </si>
+  <si>
+    <t>Se navighează la pagina de autentificare</t>
+  </si>
+  <si>
+    <t>Se afișează pagina de login</t>
+  </si>
+  <si>
+    <t>Se introduce emailul și parola în câmpurile respective</t>
+  </si>
+  <si>
+    <t>Câmpurile sunt completate corect</t>
+  </si>
+  <si>
+    <t>Se apasă pe butonul de autentificare</t>
+  </si>
+  <si>
+    <t>Se realizează autentificarea</t>
+  </si>
+  <si>
+    <t>Se măsoară timpul de încărcare post-autentificare</t>
+  </si>
+  <si>
+    <t>Redirecționare la profilul utilizatorului într-un timp satisfăcător (de exemplu, sub 4 secunde)</t>
+  </si>
+  <si>
+    <t>Utilizatorul este autentificat corect și este redirecționat către pagina de profil sau pagina principală.</t>
   </si>
 </sst>
 </file>
@@ -749,7 +845,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -963,12 +1059,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1001,13 +1134,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1019,12 +1167,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1045,6 +1187,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1054,19 +1202,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1352,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:G173"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,10 +1510,10 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="9">
         <v>1</v>
       </c>
@@ -1380,10 +1522,10 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="2:7" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="9" t="s">
         <v>28</v>
       </c>
@@ -1392,45 +1534,45 @@
       <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:7" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="22"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
     </row>
     <row r="5" spans="2:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="23" t="s">
+      <c r="B5" s="21"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="25"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
     </row>
     <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1550,10 +1692,10 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1563,10 +1705,10 @@
     </row>
     <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="16" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="9">
         <v>2</v>
       </c>
@@ -1575,10 +1717,10 @@
       <c r="G16" s="10"/>
     </row>
     <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="9" t="s">
         <v>68</v>
       </c>
@@ -1587,55 +1729,55 @@
       <c r="G17" s="10"/>
     </row>
     <row r="18" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="20" t="s">
+      <c r="C18" s="20"/>
+      <c r="D18" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="25"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="23" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
     </row>
     <row r="20" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="26" t="s">
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1755,10 +1897,10 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="30"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="9" t="s">
         <v>27</v>
       </c>
@@ -1768,10 +1910,10 @@
     </row>
     <row r="30" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="9">
         <v>3</v>
       </c>
@@ -1780,10 +1922,10 @@
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="9" t="s">
         <v>69</v>
       </c>
@@ -1792,45 +1934,45 @@
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="20" t="s">
+      <c r="C33" s="20"/>
+      <c r="D33" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="22"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="25"/>
     </row>
     <row r="34" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="23" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="30"/>
+      <c r="D36" s="12"/>
       <c r="E36" s="2" t="s">
         <v>5</v>
       </c>
@@ -1968,10 +2110,10 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="30"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="9" t="s">
         <v>37</v>
       </c>
@@ -1981,10 +2123,10 @@
     </row>
     <row r="45" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="46" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="12"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="9">
         <v>4</v>
       </c>
@@ -1993,10 +2135,10 @@
       <c r="G46" s="10"/>
     </row>
     <row r="47" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="12"/>
+      <c r="C47" s="18"/>
       <c r="D47" s="9" t="s">
         <v>70</v>
       </c>
@@ -2005,45 +2147,45 @@
       <c r="G47" s="10"/>
     </row>
     <row r="48" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="20" t="s">
+      <c r="C48" s="20"/>
+      <c r="D48" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="25"/>
     </row>
     <row r="49" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="16"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="23" t="s">
+      <c r="B49" s="21"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
+      <c r="E49" s="27"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="28"/>
     </row>
     <row r="50" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="33"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="16"/>
     </row>
     <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="30"/>
+      <c r="D51" s="12"/>
       <c r="E51" s="2" t="s">
         <v>5</v>
       </c>
@@ -2163,10 +2305,10 @@
       </c>
     </row>
     <row r="58" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="30"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="9" t="s">
         <v>45</v>
       </c>
@@ -2176,10 +2318,10 @@
     </row>
     <row r="59" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="12"/>
+      <c r="C60" s="18"/>
       <c r="D60" s="9">
         <v>5</v>
       </c>
@@ -2188,10 +2330,10 @@
       <c r="G60" s="10"/>
     </row>
     <row r="61" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="12"/>
+      <c r="C61" s="18"/>
       <c r="D61" s="9" t="s">
         <v>46</v>
       </c>
@@ -2200,45 +2342,45 @@
       <c r="G61" s="10"/>
     </row>
     <row r="62" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="15"/>
-      <c r="D62" s="20" t="s">
+      <c r="C62" s="20"/>
+      <c r="D62" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="22"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
     </row>
     <row r="63" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="16"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="23" t="s">
+      <c r="B63" s="21"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="25"/>
+      <c r="E63" s="27"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="28"/>
     </row>
     <row r="64" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="31" t="s">
+      <c r="B64" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="32"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="33"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="16"/>
     </row>
     <row r="65" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B65" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D65" s="30"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2306,10 +2448,10 @@
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="29" t="s">
+      <c r="B70" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C70" s="30"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="9" t="s">
         <v>52</v>
       </c>
@@ -2319,10 +2461,10 @@
     </row>
     <row r="71" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="72" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="12"/>
+      <c r="C72" s="18"/>
       <c r="D72" s="9">
         <v>6</v>
       </c>
@@ -2331,10 +2473,10 @@
       <c r="G72" s="10"/>
     </row>
     <row r="73" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="12"/>
+      <c r="C73" s="18"/>
       <c r="D73" s="9" t="s">
         <v>59</v>
       </c>
@@ -2343,45 +2485,45 @@
       <c r="G73" s="10"/>
     </row>
     <row r="74" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="15"/>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="20"/>
+      <c r="D74" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="22"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="25"/>
     </row>
     <row r="75" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="16"/>
-      <c r="C75" s="17"/>
-      <c r="D75" s="23" t="s">
+      <c r="B75" s="21"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E75" s="24"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="25"/>
+      <c r="E75" s="27"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="28"/>
     </row>
     <row r="76" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B76" s="31" t="s">
+      <c r="B76" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="33"/>
+      <c r="C76" s="15"/>
+      <c r="D76" s="15"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="16"/>
     </row>
     <row r="77" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="30"/>
+      <c r="D77" s="12"/>
       <c r="E77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2505,10 +2647,10 @@
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="29" t="s">
+      <c r="B86" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C86" s="30"/>
+      <c r="C86" s="12"/>
       <c r="D86" s="9" t="s">
         <v>88</v>
       </c>
@@ -2518,10 +2660,10 @@
     </row>
     <row r="87" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="12"/>
+      <c r="C88" s="18"/>
       <c r="D88" s="9">
         <v>7</v>
       </c>
@@ -2530,10 +2672,10 @@
       <c r="G88" s="10"/>
     </row>
     <row r="89" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="11" t="s">
+      <c r="B89" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="12"/>
+      <c r="C89" s="18"/>
       <c r="D89" s="9" t="s">
         <v>54</v>
       </c>
@@ -2542,45 +2684,45 @@
       <c r="G89" s="10"/>
     </row>
     <row r="90" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C90" s="15"/>
-      <c r="D90" s="20" t="s">
+      <c r="C90" s="20"/>
+      <c r="D90" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="22"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="25"/>
     </row>
     <row r="91" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B91" s="16"/>
-      <c r="C91" s="17"/>
-      <c r="D91" s="23" t="s">
+      <c r="B91" s="21"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="25"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="28"/>
     </row>
     <row r="92" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B92" s="31" t="s">
+      <c r="B92" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
-      <c r="E92" s="32"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="33"/>
+      <c r="C92" s="15"/>
+      <c r="D92" s="15"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="16"/>
     </row>
     <row r="93" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C93" s="29" t="s">
+      <c r="C93" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="30"/>
+      <c r="D93" s="12"/>
       <c r="E93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2690,10 +2832,10 @@
       <c r="G100" s="5"/>
     </row>
     <row r="101" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B101" s="29" t="s">
+      <c r="B101" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C101" s="30"/>
+      <c r="C101" s="12"/>
       <c r="D101" s="9" t="s">
         <v>56</v>
       </c>
@@ -2703,10 +2845,10 @@
     </row>
     <row r="102" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="103" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B103" s="11" t="s">
+      <c r="B103" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="12"/>
+      <c r="C103" s="18"/>
       <c r="D103" s="9">
         <v>8</v>
       </c>
@@ -2715,10 +2857,10 @@
       <c r="G103" s="10"/>
     </row>
     <row r="104" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C104" s="12"/>
+      <c r="C104" s="18"/>
       <c r="D104" s="9" t="s">
         <v>71</v>
       </c>
@@ -2727,45 +2869,45 @@
       <c r="G104" s="10"/>
     </row>
     <row r="105" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C105" s="15"/>
-      <c r="D105" s="20" t="s">
+      <c r="C105" s="20"/>
+      <c r="D105" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
-      <c r="G105" s="22"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="25"/>
     </row>
     <row r="106" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B106" s="16"/>
-      <c r="C106" s="17"/>
-      <c r="D106" s="23" t="s">
+      <c r="B106" s="21"/>
+      <c r="C106" s="22"/>
+      <c r="D106" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="25"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
+      <c r="G106" s="28"/>
     </row>
     <row r="107" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B107" s="31" t="s">
+      <c r="B107" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
-      <c r="E107" s="32"/>
-      <c r="F107" s="32"/>
-      <c r="G107" s="33"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="15"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="16"/>
     </row>
     <row r="108" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C108" s="29" t="s">
+      <c r="C108" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="30"/>
+      <c r="D108" s="12"/>
       <c r="E108" s="2" t="s">
         <v>5</v>
       </c>
@@ -2875,10 +3017,10 @@
       <c r="G115" s="5"/>
     </row>
     <row r="116" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B116" s="29" t="s">
+      <c r="B116" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C116" s="30"/>
+      <c r="C116" s="12"/>
       <c r="D116" s="9" t="s">
         <v>87</v>
       </c>
@@ -2888,10 +3030,10 @@
     </row>
     <row r="117" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="118" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C118" s="12"/>
+      <c r="C118" s="18"/>
       <c r="D118" s="9">
         <v>9</v>
       </c>
@@ -2900,10 +3042,10 @@
       <c r="G118" s="10"/>
     </row>
     <row r="119" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C119" s="12"/>
+      <c r="C119" s="18"/>
       <c r="D119" s="9" t="s">
         <v>80</v>
       </c>
@@ -2912,45 +3054,45 @@
       <c r="G119" s="10"/>
     </row>
     <row r="120" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C120" s="15"/>
-      <c r="D120" s="20" t="s">
+      <c r="C120" s="20"/>
+      <c r="D120" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
-      <c r="G120" s="22"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="25"/>
     </row>
     <row r="121" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B121" s="16"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="23" t="s">
+      <c r="B121" s="21"/>
+      <c r="C121" s="22"/>
+      <c r="D121" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E121" s="24"/>
-      <c r="F121" s="24"/>
-      <c r="G121" s="25"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="28"/>
     </row>
     <row r="122" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B122" s="31" t="s">
+      <c r="B122" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C122" s="32"/>
-      <c r="D122" s="32"/>
-      <c r="E122" s="32"/>
-      <c r="F122" s="32"/>
-      <c r="G122" s="33"/>
+      <c r="C122" s="15"/>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="16"/>
     </row>
     <row r="123" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B123" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C123" s="29" t="s">
+      <c r="C123" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D123" s="30"/>
+      <c r="D123" s="12"/>
       <c r="E123" s="2" t="s">
         <v>5</v>
       </c>
@@ -3034,10 +3176,10 @@
       </c>
     </row>
     <row r="128" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B128" s="29" t="s">
+      <c r="B128" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="30"/>
+      <c r="C128" s="12"/>
       <c r="D128" s="9" t="s">
         <v>109</v>
       </c>
@@ -3047,10 +3189,10 @@
     </row>
     <row r="129" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="130" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B130" s="11" t="s">
+      <c r="B130" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="12"/>
+      <c r="C130" s="18"/>
       <c r="D130" s="9">
         <v>10</v>
       </c>
@@ -3059,10 +3201,10 @@
       <c r="G130" s="10"/>
     </row>
     <row r="131" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B131" s="11" t="s">
+      <c r="B131" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C131" s="12"/>
+      <c r="C131" s="18"/>
       <c r="D131" s="9" t="s">
         <v>91</v>
       </c>
@@ -3071,45 +3213,45 @@
       <c r="G131" s="10"/>
     </row>
     <row r="132" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B132" s="14" t="s">
+      <c r="B132" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C132" s="15"/>
-      <c r="D132" s="20" t="s">
+      <c r="C132" s="20"/>
+      <c r="D132" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E132" s="21"/>
-      <c r="F132" s="21"/>
-      <c r="G132" s="22"/>
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="25"/>
     </row>
     <row r="133" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B133" s="16"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="23" t="s">
+      <c r="B133" s="21"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E133" s="24"/>
-      <c r="F133" s="24"/>
-      <c r="G133" s="25"/>
+      <c r="E133" s="27"/>
+      <c r="F133" s="27"/>
+      <c r="G133" s="28"/>
     </row>
     <row r="134" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B134" s="31" t="s">
+      <c r="B134" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C134" s="32"/>
-      <c r="D134" s="32"/>
-      <c r="E134" s="32"/>
-      <c r="F134" s="32"/>
-      <c r="G134" s="33"/>
+      <c r="C134" s="15"/>
+      <c r="D134" s="15"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="16"/>
     </row>
     <row r="135" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C135" s="29" t="s">
+      <c r="C135" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D135" s="30"/>
+      <c r="D135" s="12"/>
       <c r="E135" s="2" t="s">
         <v>5</v>
       </c>
@@ -3283,10 +3425,10 @@
       </c>
     </row>
     <row r="145" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B145" s="29" t="s">
+      <c r="B145" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C145" s="30"/>
+      <c r="C145" s="12"/>
       <c r="D145" s="9" t="s">
         <v>110</v>
       </c>
@@ -3296,10 +3438,10 @@
     </row>
     <row r="146" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="147" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B147" s="11" t="s">
+      <c r="B147" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C147" s="12"/>
+      <c r="C147" s="18"/>
       <c r="D147" s="9">
         <v>11</v>
       </c>
@@ -3308,10 +3450,10 @@
       <c r="G147" s="10"/>
     </row>
     <row r="148" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C148" s="12"/>
+      <c r="C148" s="18"/>
       <c r="D148" s="9" t="s">
         <v>121</v>
       </c>
@@ -3320,45 +3462,45 @@
       <c r="G148" s="10"/>
     </row>
     <row r="149" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B149" s="14" t="s">
+      <c r="B149" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C149" s="15"/>
-      <c r="D149" s="20" t="s">
+      <c r="C149" s="20"/>
+      <c r="D149" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E149" s="21"/>
-      <c r="F149" s="21"/>
-      <c r="G149" s="22"/>
+      <c r="E149" s="24"/>
+      <c r="F149" s="24"/>
+      <c r="G149" s="25"/>
     </row>
     <row r="150" spans="2:7" ht="14.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B150" s="16"/>
-      <c r="C150" s="17"/>
-      <c r="D150" s="23" t="s">
+      <c r="B150" s="21"/>
+      <c r="C150" s="22"/>
+      <c r="D150" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E150" s="24"/>
-      <c r="F150" s="24"/>
-      <c r="G150" s="25"/>
+      <c r="E150" s="27"/>
+      <c r="F150" s="27"/>
+      <c r="G150" s="28"/>
     </row>
     <row r="151" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B151" s="31" t="s">
+      <c r="B151" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C151" s="32"/>
-      <c r="D151" s="32"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="32"/>
-      <c r="G151" s="33"/>
+      <c r="C151" s="15"/>
+      <c r="D151" s="15"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="16"/>
     </row>
     <row r="152" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C152" s="29" t="s">
+      <c r="C152" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D152" s="30"/>
+      <c r="D152" s="12"/>
       <c r="E152" s="2" t="s">
         <v>5</v>
       </c>
@@ -3478,10 +3620,10 @@
       </c>
     </row>
     <row r="159" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B159" s="29" t="s">
+      <c r="B159" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C159" s="30"/>
+      <c r="C159" s="12"/>
       <c r="D159" s="9" t="s">
         <v>132</v>
       </c>
@@ -3491,10 +3633,10 @@
     </row>
     <row r="160" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="161" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B161" s="11" t="s">
+      <c r="B161" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C161" s="12"/>
+      <c r="C161" s="18"/>
       <c r="D161" s="9">
         <v>12</v>
       </c>
@@ -3503,10 +3645,10 @@
       <c r="G161" s="10"/>
     </row>
     <row r="162" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B162" s="11" t="s">
+      <c r="B162" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C162" s="12"/>
+      <c r="C162" s="18"/>
       <c r="D162" s="9" t="s">
         <v>111</v>
       </c>
@@ -3515,45 +3657,45 @@
       <c r="G162" s="10"/>
     </row>
     <row r="163" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B163" s="14" t="s">
+      <c r="B163" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C163" s="15"/>
-      <c r="D163" s="20" t="s">
+      <c r="C163" s="20"/>
+      <c r="D163" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E163" s="21"/>
-      <c r="F163" s="21"/>
-      <c r="G163" s="22"/>
+      <c r="E163" s="24"/>
+      <c r="F163" s="24"/>
+      <c r="G163" s="25"/>
     </row>
     <row r="164" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B164" s="16"/>
-      <c r="C164" s="17"/>
-      <c r="D164" s="23" t="s">
+      <c r="B164" s="21"/>
+      <c r="C164" s="22"/>
+      <c r="D164" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E164" s="24"/>
-      <c r="F164" s="24"/>
-      <c r="G164" s="25"/>
+      <c r="E164" s="27"/>
+      <c r="F164" s="27"/>
+      <c r="G164" s="28"/>
     </row>
     <row r="165" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B165" s="31" t="s">
+      <c r="B165" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C165" s="32"/>
-      <c r="D165" s="32"/>
-      <c r="E165" s="32"/>
-      <c r="F165" s="32"/>
-      <c r="G165" s="33"/>
+      <c r="C165" s="15"/>
+      <c r="D165" s="15"/>
+      <c r="E165" s="15"/>
+      <c r="F165" s="15"/>
+      <c r="G165" s="16"/>
     </row>
     <row r="166" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B166" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C166" s="29" t="s">
+      <c r="C166" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D166" s="30"/>
+      <c r="D166" s="12"/>
       <c r="E166" s="2" t="s">
         <v>5</v>
       </c>
@@ -3655,10 +3797,10 @@
       </c>
     </row>
     <row r="172" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B172" s="29" t="s">
+      <c r="B172" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C172" s="30"/>
+      <c r="C172" s="12"/>
       <c r="D172" s="9" t="s">
         <v>120</v>
       </c>
@@ -3669,6 +3811,190 @@
     <row r="173" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="208">
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="B18:C20"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:G32"/>
+    <mergeCell ref="B33:C34"/>
+    <mergeCell ref="D33:G33"/>
+    <mergeCell ref="D34:G34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="D172:G172"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C157:D157"/>
+    <mergeCell ref="C158:D158"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="D161:G161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:G162"/>
+    <mergeCell ref="B163:C164"/>
+    <mergeCell ref="D163:G163"/>
+    <mergeCell ref="D164:G164"/>
+    <mergeCell ref="B165:G165"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C155:D155"/>
+    <mergeCell ref="C156:D156"/>
+    <mergeCell ref="B159:C159"/>
+    <mergeCell ref="D159:G159"/>
+    <mergeCell ref="B151:G151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="D145:G145"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:G147"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="C143:D143"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:G148"/>
+    <mergeCell ref="B149:C150"/>
+    <mergeCell ref="D149:G149"/>
+    <mergeCell ref="D150:G150"/>
+    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="D128:G128"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="D130:G130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:G131"/>
+    <mergeCell ref="B132:C133"/>
+    <mergeCell ref="D132:G132"/>
+    <mergeCell ref="D133:G133"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:G119"/>
+    <mergeCell ref="B120:C121"/>
+    <mergeCell ref="D120:G120"/>
+    <mergeCell ref="D121:G121"/>
+    <mergeCell ref="B122:G122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:G118"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:G44"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:G47"/>
+    <mergeCell ref="B48:C49"/>
+    <mergeCell ref="D48:G48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:G61"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D63:G63"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D60:G60"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="B74:C75"/>
+    <mergeCell ref="D74:G74"/>
+    <mergeCell ref="D75:G75"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:G89"/>
+    <mergeCell ref="B90:C91"/>
+    <mergeCell ref="D90:G90"/>
+    <mergeCell ref="D91:G91"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D88:G88"/>
     <mergeCell ref="C115:D115"/>
     <mergeCell ref="B116:C116"/>
     <mergeCell ref="D116:G116"/>
@@ -3693,190 +4019,6 @@
     <mergeCell ref="C93:D93"/>
     <mergeCell ref="C94:D94"/>
     <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:G89"/>
-    <mergeCell ref="B90:C91"/>
-    <mergeCell ref="D90:G90"/>
-    <mergeCell ref="D91:G91"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="B76:G76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="B74:C75"/>
-    <mergeCell ref="D74:G74"/>
-    <mergeCell ref="D75:G75"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:G70"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:G72"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:G61"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D63:G63"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:G58"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:G60"/>
-    <mergeCell ref="B50:G50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="B48:C49"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="D29:G29"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:G118"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:G16"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:G119"/>
-    <mergeCell ref="B120:C121"/>
-    <mergeCell ref="D120:G120"/>
-    <mergeCell ref="D121:G121"/>
-    <mergeCell ref="B122:G122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="D148:G148"/>
-    <mergeCell ref="B149:C150"/>
-    <mergeCell ref="D149:G149"/>
-    <mergeCell ref="D150:G150"/>
-    <mergeCell ref="C126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="D128:G128"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="D130:G130"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="D131:G131"/>
-    <mergeCell ref="B132:C133"/>
-    <mergeCell ref="D132:G132"/>
-    <mergeCell ref="D133:G133"/>
-    <mergeCell ref="C155:D155"/>
-    <mergeCell ref="C156:D156"/>
-    <mergeCell ref="B159:C159"/>
-    <mergeCell ref="D159:G159"/>
-    <mergeCell ref="B151:G151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="B145:C145"/>
-    <mergeCell ref="D145:G145"/>
-    <mergeCell ref="B147:C147"/>
-    <mergeCell ref="D147:G147"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="C143:D143"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="C168:D168"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="C170:D170"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="D172:G172"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="C157:D157"/>
-    <mergeCell ref="C158:D158"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="D161:G161"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="D162:G162"/>
-    <mergeCell ref="B163:C164"/>
-    <mergeCell ref="D163:G163"/>
-    <mergeCell ref="D164:G164"/>
-    <mergeCell ref="B165:G165"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="B18:C20"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:C34"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3884,10 +4026,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E192BF06-66C7-4B4F-95C1-D1A93166083F}">
-  <dimension ref="B4:G58"/>
+  <dimension ref="B1:G108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3899,803 +4041,1557 @@
     <col min="6" max="6" width="33.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="11" t="s">
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="9">
-        <v>9</v>
-      </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="9">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="29"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
     </row>
     <row r="6" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
-    </row>
-    <row r="7" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="C8" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="33"/>
+      <c r="C9" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>66</v>
+        <v>222</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="25"/>
+    </row>
+    <row r="17" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="36"/>
+    </row>
+    <row r="18" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="3">
+        <v>4</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="3">
+        <v>5</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="9">
+        <v>3</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="36"/>
+    </row>
+    <row r="31" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="10"/>
+      <c r="E34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" s="10"/>
+      <c r="E35" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="3">
+        <v>4</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D36" s="10"/>
+      <c r="E36" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="3">
+        <v>5</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D37" s="10"/>
+      <c r="E37" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="9">
+        <v>4</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="20"/>
+      <c r="D42" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="25"/>
+    </row>
+    <row r="43" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="36"/>
+    </row>
+    <row r="44" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="16"/>
+    </row>
+    <row r="45" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="3">
+        <v>3</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="3">
+        <v>4</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="3">
+        <v>5</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="9">
+        <v>9</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="2:7" ht="15.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="25"/>
+    </row>
+    <row r="58" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="29"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="36"/>
+    </row>
+    <row r="59" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="16"/>
+    </row>
+    <row r="60" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" s="12"/>
+      <c r="E60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="3">
+        <v>1</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F61" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="3">
+      <c r="G61" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C62" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="4" t="s">
+      <c r="D62" s="10"/>
+      <c r="E62" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F62" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="37.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="3">
+      <c r="G62" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="37.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C63" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="4" t="s">
+      <c r="D63" s="10"/>
+      <c r="E63" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F63" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="3">
+      <c r="G63" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C64" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="4" t="s">
+      <c r="D64" s="10"/>
+      <c r="E64" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F64" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="3">
+      <c r="G64" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="43.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="4" t="s">
+      <c r="D65" s="10"/>
+      <c r="E65" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F65" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="34.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="3">
+      <c r="G65" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="34.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="3">
         <v>6</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="4" t="s">
+      <c r="D66" s="10"/>
+      <c r="E66" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F66" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="29" t="s">
+      <c r="G66" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="9" t="s">
+      <c r="C67" s="12"/>
+      <c r="D67" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="11" t="s">
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="69" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="12"/>
-      <c r="D19" s="9">
+      <c r="C69" s="18"/>
+      <c r="D69" s="9">
         <v>10</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="11" t="s">
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="10"/>
+    </row>
+    <row r="70" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B70" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="9" t="s">
+      <c r="C70" s="18"/>
+      <c r="D70" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="10"/>
+    </row>
+    <row r="71" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="20" t="s">
+      <c r="C71" s="20"/>
+      <c r="D71" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="23" t="s">
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="25"/>
+    </row>
+    <row r="72" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B72" s="21"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="31" t="s">
+      <c r="E72" s="27"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="28"/>
+    </row>
+    <row r="73" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B73" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-    </row>
-    <row r="24" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="16"/>
+    </row>
+    <row r="74" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C74" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="2" t="s">
+      <c r="D74" s="12"/>
+      <c r="E74" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="45.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="3">
+    <row r="75" spans="2:7" ht="45.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="3">
         <v>1</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C75" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="4" t="s">
+      <c r="D75" s="10"/>
+      <c r="E75" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F75" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="37.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="3">
+      <c r="G75" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="37.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B76" s="3">
         <v>2</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C76" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="4" t="s">
+      <c r="D76" s="10"/>
+      <c r="E76" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F76" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="3">
+      <c r="G76" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B77" s="3">
         <v>3</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C77" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="4" t="s">
+      <c r="D77" s="10"/>
+      <c r="E77" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F77" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="G27" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="29.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="3">
+      <c r="G77" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="29.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B78" s="3">
         <v>4</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C78" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="4" t="s">
+      <c r="D78" s="10"/>
+      <c r="E78" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="F78" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G28" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="31.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="3">
+      <c r="G78" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="31.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B79" s="3">
         <v>5</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C79" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="4" t="s">
+      <c r="D79" s="10"/>
+      <c r="E79" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="4" t="s">
+      <c r="F79" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G29" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="29" t="s">
+      <c r="G79" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B80" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="9" t="s">
+      <c r="C80" s="12"/>
+      <c r="D80" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="11" t="s">
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="10"/>
+    </row>
+    <row r="81" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="82" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B82" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="9">
+      <c r="C82" s="18"/>
+      <c r="D82" s="9">
         <v>11</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="11" t="s">
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B83" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="12"/>
-      <c r="D33" s="9" t="s">
+      <c r="C83" s="18"/>
+      <c r="D83" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="14" t="s">
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B84" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="20" t="s">
+      <c r="C84" s="20"/>
+      <c r="D84" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="22"/>
-    </row>
-    <row r="35" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="20" t="s">
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="25"/>
+    </row>
+    <row r="85" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="22"/>
-    </row>
-    <row r="36" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="23" t="s">
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="25"/>
+    </row>
+    <row r="86" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B86" s="29"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="25"/>
-    </row>
-    <row r="37" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="31" t="s">
+      <c r="E86" s="27"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="28"/>
+    </row>
+    <row r="87" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B87" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-    </row>
-    <row r="38" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="1" t="s">
+      <c r="C87" s="15"/>
+      <c r="D87" s="15"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="16"/>
+    </row>
+    <row r="88" spans="2:7" ht="39.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B88" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C88" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="30"/>
-      <c r="E38" s="2" t="s">
+      <c r="D88" s="12"/>
+      <c r="E88" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G88" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="3">
+    <row r="89" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B89" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C89" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="4" t="s">
+      <c r="D89" s="10"/>
+      <c r="E89" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F89" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="3">
+      <c r="G89" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B90" s="3">
         <v>2</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C90" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="4" t="s">
+      <c r="D90" s="10"/>
+      <c r="E90" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F90" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" ht="39.450000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="3">
+      <c r="G90" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" ht="39.450000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B91" s="3">
         <v>3</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C91" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D41" s="10"/>
-      <c r="E41" s="4" t="s">
+      <c r="D91" s="10"/>
+      <c r="E91" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F91" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" ht="40.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="3">
+      <c r="G91" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="40.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B92" s="3">
         <v>4</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C92" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="4" t="s">
+      <c r="D92" s="10"/>
+      <c r="E92" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F92" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="3">
+      <c r="G92" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="51.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B93" s="3">
         <v>5</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C93" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="D43" s="10"/>
-      <c r="E43" s="4" t="s">
+      <c r="D93" s="10"/>
+      <c r="E93" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F93" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="29" t="s">
+      <c r="G93" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B94" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="9" t="s">
+      <c r="C94" s="12"/>
+      <c r="D94" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="10"/>
-    </row>
-    <row r="45" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="11" t="s">
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="10"/>
+    </row>
+    <row r="95" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="9">
+      <c r="C96" s="18"/>
+      <c r="D96" s="9">
         <v>12</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="10"/>
-    </row>
-    <row r="47" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="11" t="s">
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="10"/>
+    </row>
+    <row r="97" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B97" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="9" t="s">
+      <c r="C97" s="18"/>
+      <c r="D97" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="10"/>
-    </row>
-    <row r="48" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="14" t="s">
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="10"/>
+    </row>
+    <row r="98" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="20" t="s">
+      <c r="C98" s="20"/>
+      <c r="D98" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="22"/>
-    </row>
-    <row r="49" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="16"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="20" t="s">
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="25"/>
+    </row>
+    <row r="99" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="21"/>
+      <c r="C99" s="22"/>
+      <c r="D99" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
-    </row>
-    <row r="50" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="18"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="23" t="s">
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="25"/>
+    </row>
+    <row r="100" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B100" s="29"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="25"/>
-    </row>
-    <row r="51" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="31" t="s">
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="28"/>
+    </row>
+    <row r="101" spans="2:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B101" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="32"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="33"/>
-    </row>
-    <row r="52" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="1" t="s">
+      <c r="C101" s="15"/>
+      <c r="D101" s="15"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="16"/>
+    </row>
+    <row r="102" spans="2:7" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C102" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D52" s="30"/>
-      <c r="E52" s="2" t="s">
+      <c r="D102" s="12"/>
+      <c r="E102" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="3">
+    <row r="103" spans="2:7" ht="30.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="3">
         <v>1</v>
       </c>
-      <c r="C53" s="9" t="s">
+      <c r="C103" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="10"/>
-      <c r="E53" s="4" t="s">
+      <c r="D103" s="10"/>
+      <c r="E103" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F53" s="4" t="s">
+      <c r="F103" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G53" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="54" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="3">
+      <c r="G103" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="3">
         <v>2</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C104" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D54" s="10"/>
-      <c r="E54" s="4" t="s">
+      <c r="D104" s="10"/>
+      <c r="E104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F104" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="G54" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="3">
+      <c r="G104" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="3">
         <v>3</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C105" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="4" t="s">
+      <c r="D105" s="10"/>
+      <c r="E105" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F105" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="G55" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="54.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="3">
+      <c r="G105" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" ht="54.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="3">
         <v>4</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C106" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="4" t="s">
+      <c r="D106" s="10"/>
+      <c r="E106" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F106" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="G56" s="8" t="s">
+      <c r="G106" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="2:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="29" t="s">
+    <row r="107" spans="2:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="9" t="s">
+      <c r="C107" s="12"/>
+      <c r="D107" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="10"/>
-    </row>
-    <row r="58" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="10"/>
+    </row>
+    <row r="108" spans="2:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="B57:C57"/>
+  <mergeCells count="129">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:G51"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:G41"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D43:G43"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:G28"/>
+    <mergeCell ref="B29:C30"/>
+    <mergeCell ref="D29:G29"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:G25"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:G55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="B57:C58"/>
     <mergeCell ref="D57:G57"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:G47"/>
-    <mergeCell ref="B48:C50"/>
-    <mergeCell ref="D48:G48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="D50:G50"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:G44"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:G33"/>
-    <mergeCell ref="B34:C36"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="D36:G36"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:G21"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="D58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:G67"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:G69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:G70"/>
+    <mergeCell ref="B71:C72"/>
+    <mergeCell ref="D71:G71"/>
+    <mergeCell ref="D72:G72"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:G80"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:G83"/>
+    <mergeCell ref="B84:C86"/>
+    <mergeCell ref="D84:G84"/>
+    <mergeCell ref="D85:G85"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:G94"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:G96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:G97"/>
+    <mergeCell ref="B98:C100"/>
+    <mergeCell ref="D98:G98"/>
+    <mergeCell ref="D99:G99"/>
+    <mergeCell ref="D100:G100"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="D107:G107"/>
+    <mergeCell ref="B101:G101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>